<commit_message>
Almost finish initial exclusion
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="1146">
   <si>
     <t xml:space="preserve">Material search results</t>
   </si>
@@ -2780,6 +2780,9 @@
     <t xml:space="preserve">10.1007/978-3-319-41649-6_20</t>
   </si>
   <si>
+    <t xml:space="preserve">Logical uncertainty</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expression Graphs</t>
   </si>
   <si>
@@ -2798,6 +2801,9 @@
     <t xml:space="preserve">10.1007/978-3-319-21365-1_25</t>
   </si>
   <si>
+    <t xml:space="preserve">Factor graphs, Bayesian networks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lifelong Learning Starting from Zero</t>
   </si>
   <si>
@@ -2816,6 +2822,9 @@
     <t xml:space="preserve">10.1007/978-3-030-27005-6_19</t>
   </si>
   <si>
+    <t xml:space="preserve">Deep learning, neural networks</t>
+  </si>
+  <si>
     <t xml:space="preserve">An Information-Theoretic Predictive Model for the Accuracy of AI Agents Adapted from Psychometrics</t>
   </si>
   <si>
@@ -2831,6 +2840,9 @@
     <t xml:space="preserve">10.1007/978-3-319-63703-7_21</t>
   </si>
   <si>
+    <t xml:space="preserve">Agent evaluation</t>
+  </si>
+  <si>
     <t xml:space="preserve">A Computational Theory for Life-Long Learning of Semantics</t>
   </si>
   <si>
@@ -2849,6 +2861,9 @@
     <t xml:space="preserve">10.1007/978-3-319-97676-1_21</t>
   </si>
   <si>
+    <t xml:space="preserve">Semantic vectors, semantic communication</t>
+  </si>
+  <si>
     <t xml:space="preserve">Partial Operator Induction with Beta Distributions</t>
   </si>
   <si>
@@ -2867,6 +2882,9 @@
     <t xml:space="preserve">10.1007/978-3-319-97676-1_6</t>
   </si>
   <si>
+    <t xml:space="preserve">Solomonoff operator induction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Decision-Making During Language Understanding by Intelligent Agents</t>
   </si>
   <si>
@@ -2885,6 +2903,9 @@
     <t xml:space="preserve">10.1007/978-3-319-21365-1_32</t>
   </si>
   <si>
+    <t xml:space="preserve">NL understanding, reasoning, OntoAgents</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anchoring Knowledge in Interaction: Towards a Harmonic Subsymbolic/Symbolic Framework and Architecture of Computational Cognition</t>
   </si>
   <si>
@@ -2903,14 +2924,16 @@
     <t xml:space="preserve">10.1007/978-3-319-21365-1_4</t>
   </si>
   <si>
+    <t xml:space="preserve">Transfer learning, architecture</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extending MicroPsi’s Model of Motivation and Emotion for Conversational Agents</t>
   </si>
   <si>
     <t xml:space="preserve">Joscha BachMurilo CoutinhoLiza Lichtinger</t>
   </si>
   <si>
-    <t xml:space="preserve">We describe a model of emotion and motivation that extends the MicroPsi motivation model for applications in conversational agents and tracking human emotions. The model is based on reactions of the agent to satisfaction and frustration of physiological, cognitive or social needs, and to changes of the agent’s expectations regarding such events. The model covers motivational states, affective states (modulation of cognition), feelings (sensations that correspond to a situation appraisal), emotions (conceptual aggregates of motivational states, modulators and feelings) and is currently being adapted to express emotional states.
-</t>
+    <t xml:space="preserve">We describe a model of emotion and motivation that extends the MicroPsi motivation model for applications in conversational agents and tracking human emotions. The model is based on reactions of the agent to satisfaction and frustration of physiological, cognitive or social needs, and to changes of the agent’s expectations regarding such events. The model covers motivational states, affective states (modulation of cognition), feelings (sensations that correspond to a situation appraisal), emotions (conceptual aggregates of motivational states, modulators and feelings) and is currently being adapted to express emotional states.</t>
   </si>
   <si>
     <t xml:space="preserve">MicroPsi architecture, Artificial emotion, Affect, Motivation, Modulation, Feelings, Appraisal models, Affective computing</t>
@@ -2922,6 +2945,9 @@
     <t xml:space="preserve">10.1007/978-3-030-27005-6_4</t>
   </si>
   <si>
+    <t xml:space="preserve">Micropsi architecture, artificial emotion</t>
+  </si>
+  <si>
     <t xml:space="preserve">What People Say? Web-Based Casuistry for Artificial Morality Experiments</t>
   </si>
   <si>
@@ -2937,6 +2963,9 @@
     <t xml:space="preserve">10.1007/978-3-319-63703-7_17</t>
   </si>
   <si>
+    <t xml:space="preserve">Machine morality, agent ethics</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two Attempts to Formalize Counterpossible Reasoning in Deterministic Settings</t>
   </si>
   <si>
@@ -2973,6 +3002,9 @@
     <t xml:space="preserve">10.1007/978-3-319-21365-1_29</t>
   </si>
   <si>
+    <t xml:space="preserve">Grid cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan Recovery in Reactive HTNs Using Symbolic Planning</t>
   </si>
   <si>
@@ -2991,6 +3023,9 @@
     <t xml:space="preserve">10.1007/978-3-319-21365-1_33</t>
   </si>
   <si>
+    <t xml:space="preserve">Symbolic modeling, agent planning</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zeta Distribution and Transfer Learning Problem</t>
   </si>
   <si>
@@ -3003,14 +3038,16 @@
     <t xml:space="preserve">10.1007/978-3-319-97676-1_17</t>
   </si>
   <si>
+    <t xml:space="preserve">Transfer learning, zeta distribution</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orthogonality-Based Disentanglement of Responsibilities for Ethical Intelligent Systems</t>
   </si>
   <si>
     <t xml:space="preserve">Nadisha-Marie AlimanLeon KesterPeter WerkhovenRoman Yampolskiy</t>
   </si>
   <si>
-    <t xml:space="preserve">In recent years, the implementation of meaningfully controllable advanced intelligent systems whose goals are aligned with ethical values as specified by human entities emerged as key subject of investigation of international relevance across diverse AI-related research areas. In this paper, we present a novel transdisciplinary and Systems Engineering oriented approach denoted “orthogonality-based disentanglement” which jointly tackles both the thereby underlying control problem and value alignment problem while unraveling the corresponding responsibilities of different stakeholders based on the distinction of two orthogonal axes assigned to the problem-solving ability of these intelligent systems on the one hand and to the ethical abilities they exhibit based on quantitatively encoded human values on the other hand. Moreover, we introduce the notion of explicitly formulated ethical goal functions ideally encoding what humans should want and exemplify a possible class of “self-aware” intelligent systems with the capability to reliably adhere to these human-defined goal functions. Beyond that, we discuss an attainable transformative socio-technological feedback-loop that could result out of the introduced orthogonality-based disentanglement approach and briefly elaborate on how the framework additionally provides valuable hints with regard to the coordination subtask in AI Safety. Finally, we point out remaining crucial challenges as incentive for future work.
-</t>
+    <t xml:space="preserve">In recent years, the implementation of meaningfully controllable advanced intelligent systems whose goals are aligned with ethical values as specified by human entities emerged as key subject of investigation of international relevance across diverse AI-related research areas. In this paper, we present a novel transdisciplinary and Systems Engineering oriented approach denoted “orthogonality-based disentanglement” which jointly tackles both the thereby underlying control problem and value alignment problem while unraveling the corresponding responsibilities of different stakeholders based on the distinction of two orthogonal axes assigned to the problem-solving ability of these intelligent systems on the one hand and to the ethical abilities they exhibit based on quantitatively encoded human values on the other hand. Moreover, we introduce the notion of explicitly formulated ethical goal functions ideally encoding what humans should want and exemplify a possible class of “self-aware” intelligent systems with the capability to reliably adhere to these human-defined goal functions. Beyond that, we discuss an attainable transformative socio-technological feedback-loop that could result out of the introduced orthogonality-based disentanglement approach and briefly elaborate on how the framework additionally provides valuable hints with regard to the coordination subtask in AI Safety. Finally, we point out remaining crucial challenges as incentive for future work.</t>
   </si>
   <si>
     <t xml:space="preserve">Ethical goal function, Self-awareness, AI alignment, Control problem, AI coordination</t>
@@ -3028,8 +3065,7 @@
     <t xml:space="preserve">Paul S. RosenbloomAbram DemskiVolkan Ustun</t>
   </si>
   <si>
-    <t xml:space="preserve">The status of Sigma’s grounding in graphical models is challenged by the ways in which their semantics has been violated while incorporating rule-based reasoning into them. This has led to a rethinking of what goes on in its graphical architecture, with results that include a straightforward extension to feedforward neural networks (although not yet with learning).
-</t>
+    <t xml:space="preserve">The status of Sigma’s grounding in graphical models is challenged by the ways in which their semantics has been violated while incorporating rule-based reasoning into them. This has led to a rethinking of what goes on in its graphical architecture, with results that include a straightforward extension to feedforward neural networks (although not yet with learning).</t>
   </si>
   <si>
     <t xml:space="preserve">Cognitive architecture, Graphical models, Neural network</t>
@@ -3077,15 +3113,16 @@
     <t xml:space="preserve">10.1007/978-3-319-41649-6_30</t>
   </si>
   <si>
+    <t xml:space="preserve">Cartesian compression, deep learning</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cognitive Module Networks for Grounded Reasoning</t>
   </si>
   <si>
     <t xml:space="preserve">Alexey PotapovAnatoly BelikovVitaly BogdanovAlexander Scherbatiy</t>
   </si>
   <si>
-    <t xml:space="preserve">
-The necessity for neural-symbolic integration becomes evident as more complex problems like visual question answering are beginning to be addressed, which go beyond such limited-domain tasks as classification. Many existing state-of-the-art models are designed for a particular task or even benchmark, while general-purpose approaches are rarely applied to a wide variety of tasks demonstrating high performance. We propose a hybrid neural-symbolic framework, which tightly integrates the knowledge representation and symbolic reasoning mechanisms of the OpenCog cognitive architecture and one of the contemporary deep learning libraries, PyTorch, and show how to implement some existing particular models in our general framework.
-</t>
+    <t xml:space="preserve">The necessity for neural-symbolic integration becomes evident as more complex problems like visual question answering are beginning to be addressed, which go beyond such limited-domain tasks as classification. Many existing state-of-the-art models are designed for a particular task or even benchmark, while general-purpose approaches are rarely applied to a wide variety of tasks demonstrating high performance. We propose a hybrid neural-symbolic framework, which tightly integrates the knowledge representation and symbolic reasoning mechanisms of the OpenCog cognitive architecture and one of the contemporary deep learning libraries, PyTorch, and show how to implement some existing particular models in our general framework.</t>
   </si>
   <si>
     <t xml:space="preserve">Grounded reasoning, Cognitive architectures, Neural module networks, Visual question answering</t>
@@ -3103,8 +3140,7 @@
     <t xml:space="preserve">Roman VisotskyYuval AtzmonGal Chechik</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Learning from few samples is a major challenge for parameter-rich models such as deep networks. In contrast, people can learn complex new concepts even from very few examples, suggesting that the sample complexity of learning can often be reduced. We describe an approach to reduce the number of samples needed for learning using per-sample side information. Specifically, we show how to speed up learning by providing textual information about feature relevance, like the presence of objects in a scene or attributes in an image. We also give an improved generalization error bound for this case. We formulate the learning problem using an ellipsoid-margin loss, and develop an algorithm that minimizes this loss effectively. Empirical evaluation on two machine vision benchmarks for scene classification and fine-grain bird classification demonstrate the benefits of this approach for few-shot learning.</t>
+    <t xml:space="preserve">Learning from few samples is a major challenge for parameter-rich models such as deep networks. In contrast, people can learn complex new concepts even from very few examples, suggesting that the sample complexity of learning can often be reduced. We describe an approach to reduce the number of samples needed for learning using per-sample side information. Specifically, we show how to speed up learning by providing textual information about feature relevance, like the presence of objects in a scene or attributes in an image. We also give an improved generalization error bound for this case. We formulate the learning problem using an ellipsoid-margin loss, and develop an algorithm that minimizes this loss effectively. Empirical evaluation on two machine vision benchmarks for scene classification and fine-grain bird classification demonstrate the benefits of this approach for few-shot learning.</t>
   </si>
   <si>
     <t xml:space="preserve">Few-shot learning, Side information, Machine teaching</t>
@@ -3116,6 +3152,9 @@
     <t xml:space="preserve">10.1007/978-3-030-27005-6_21</t>
   </si>
   <si>
+    <t xml:space="preserve">Neural networks, side information</t>
+  </si>
+  <si>
     <t xml:space="preserve">A Time-Critical Simulation of Language Comprehension</t>
   </si>
   <si>
@@ -3134,6 +3173,9 @@
     <t xml:space="preserve">10.1007/978-3-319-97676-1_27</t>
   </si>
   <si>
+    <t xml:space="preserve">Language processing, on-line learning</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bandit Models of Human Behavior: Reward Processing in Mental Disorders</t>
   </si>
   <si>
@@ -3149,6 +3191,9 @@
     <t xml:space="preserve">10.1007/978-3-319-63703-7_22</t>
   </si>
   <si>
+    <t xml:space="preserve">Multi-armed bandit, general parametric framework</t>
+  </si>
+  <si>
     <t xml:space="preserve">Request Confirmation Networks in MicroPsi 2</t>
   </si>
   <si>
@@ -3165,6 +3210,9 @@
   </si>
   <si>
     <t xml:space="preserve">10.1007/978-3-319-97676-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micropsi architecture, neurosymbolic represention</t>
   </si>
   <si>
     <t xml:space="preserve">Associative Memory: An Spiking Neural Network Robotic Implementation</t>
@@ -3611,6 +3659,12 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
@@ -3630,12 +3684,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="33">
@@ -3659,7 +3707,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="30" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3691,7 +3739,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3723,7 +3771,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3735,7 +3783,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3743,11 +3791,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="30" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="28" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="31" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3783,14 +3831,14 @@
     <cellStyle name="Bad 2" xfId="21"/>
     <cellStyle name="Bad 3" xfId="22"/>
     <cellStyle name="Bad 4" xfId="23"/>
-    <cellStyle name="Good 1" xfId="24"/>
-    <cellStyle name="Good 2" xfId="25"/>
-    <cellStyle name="Good 3" xfId="26"/>
-    <cellStyle name="Heading 1 1" xfId="27"/>
-    <cellStyle name="Heading 1 2" xfId="28"/>
-    <cellStyle name="Heading 2 1" xfId="29"/>
-    <cellStyle name="Good" xfId="30"/>
-    <cellStyle name="Bad" xfId="31"/>
+    <cellStyle name="Bad 5" xfId="24"/>
+    <cellStyle name="Good 1" xfId="25"/>
+    <cellStyle name="Good 2" xfId="26"/>
+    <cellStyle name="Good 3" xfId="27"/>
+    <cellStyle name="Good 4" xfId="28"/>
+    <cellStyle name="Heading 1 1" xfId="29"/>
+    <cellStyle name="Heading 1 2" xfId="30"/>
+    <cellStyle name="Heading 2 1" xfId="31"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3862,11 +3910,11 @@
   </sheetPr>
   <dimension ref="A1:R191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G121" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P148" activeCellId="0" sqref="P148"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B176" activeCellId="0" sqref="B176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="111.61"/>
@@ -9891,16 +9939,22 @@
       <c r="M152" s="0" t="s">
         <v>241</v>
       </c>
+      <c r="O152" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" s="0" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="n">
         <v>151</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>2015</v>
@@ -9909,22 +9963,28 @@
         <v>236</v>
       </c>
       <c r="F153" s="12" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="G153" s="0" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H153" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M153" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O153" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" s="0" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9932,10 +9992,10 @@
         <v>152</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>2019</v>
@@ -9944,22 +10004,28 @@
         <v>236</v>
       </c>
       <c r="F154" s="12" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="G154" s="0" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="H154" s="0" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="K154" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M154" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O154" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" s="0" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9967,10 +10033,10 @@
         <v>153</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>2017</v>
@@ -9979,19 +10045,25 @@
         <v>236</v>
       </c>
       <c r="F155" s="12" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="H155" s="0" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="K155" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M155" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O155" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" s="0" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9999,10 +10071,10 @@
         <v>154</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>2018</v>
@@ -10011,22 +10083,28 @@
         <v>236</v>
       </c>
       <c r="F156" s="12" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="G156" s="0" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="H156" s="0" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="K156" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M156" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O156" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" s="0" t="s">
+        <v>946</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10034,10 +10112,10 @@
         <v>155</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>2018</v>
@@ -10046,22 +10124,28 @@
         <v>236</v>
       </c>
       <c r="F157" s="12" t="s">
-        <v>944</v>
+        <v>949</v>
       </c>
       <c r="G157" s="0" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
       <c r="H157" s="0" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>947</v>
+        <v>952</v>
       </c>
       <c r="K157" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M157" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O157" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" s="0" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10069,10 +10153,10 @@
         <v>156</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>949</v>
+        <v>955</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>2015</v>
@@ -10081,22 +10165,28 @@
         <v>236</v>
       </c>
       <c r="F158" s="12" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="G158" s="0" t="s">
-        <v>951</v>
+        <v>957</v>
       </c>
       <c r="H158" s="0" t="s">
-        <v>952</v>
+        <v>958</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>953</v>
+        <v>959</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M158" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O158" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q158" s="0" t="s">
+        <v>960</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10104,10 +10194,10 @@
         <v>157</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>2015</v>
@@ -10116,22 +10206,28 @@
         <v>236</v>
       </c>
       <c r="F159" s="12" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="G159" s="0" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
       <c r="H159" s="0" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="K159" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M159" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O159" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" s="0" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10139,10 +10235,10 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>960</v>
+        <v>968</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>961</v>
+        <v>969</v>
       </c>
       <c r="D160" s="0" t="n">
         <v>2019</v>
@@ -10151,22 +10247,28 @@
         <v>236</v>
       </c>
       <c r="F160" s="22" t="s">
-        <v>962</v>
+        <v>970</v>
       </c>
       <c r="G160" s="0" t="s">
-        <v>963</v>
+        <v>971</v>
       </c>
       <c r="H160" s="0" t="s">
-        <v>964</v>
+        <v>972</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>965</v>
+        <v>973</v>
       </c>
       <c r="K160" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M160" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O160" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="0" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10174,10 +10276,10 @@
         <v>159</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>966</v>
+        <v>975</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>967</v>
+        <v>976</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>2017</v>
@@ -10186,19 +10288,25 @@
         <v>236</v>
       </c>
       <c r="F161" s="12" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
       <c r="H161" s="0" t="s">
-        <v>969</v>
+        <v>978</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>970</v>
+        <v>979</v>
       </c>
       <c r="K161" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M161" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q161" s="0" t="s">
+        <v>980</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10206,10 +10314,10 @@
         <v>160</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>972</v>
+        <v>982</v>
       </c>
       <c r="D162" s="0" t="n">
         <v>2015</v>
@@ -10218,22 +10326,25 @@
         <v>236</v>
       </c>
       <c r="F162" s="12" t="s">
-        <v>973</v>
+        <v>983</v>
       </c>
       <c r="G162" s="0" t="s">
-        <v>974</v>
+        <v>984</v>
       </c>
       <c r="H162" s="0" t="s">
-        <v>975</v>
+        <v>985</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>976</v>
+        <v>986</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M162" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O162" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10241,10 +10352,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>977</v>
+        <v>987</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>978</v>
+        <v>988</v>
       </c>
       <c r="D163" s="0" t="n">
         <v>2015</v>
@@ -10253,22 +10364,28 @@
         <v>236</v>
       </c>
       <c r="F163" s="12" t="s">
-        <v>979</v>
+        <v>989</v>
       </c>
       <c r="G163" s="0" t="s">
-        <v>980</v>
+        <v>990</v>
       </c>
       <c r="H163" s="0" t="s">
-        <v>981</v>
+        <v>991</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>982</v>
+        <v>992</v>
       </c>
       <c r="K163" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M163" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="0" t="s">
+        <v>993</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10276,10 +10393,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>983</v>
+        <v>994</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>984</v>
+        <v>995</v>
       </c>
       <c r="D164" s="0" t="n">
         <v>2015</v>
@@ -10288,22 +10405,28 @@
         <v>236</v>
       </c>
       <c r="F164" s="12" t="s">
-        <v>985</v>
+        <v>996</v>
       </c>
       <c r="G164" s="0" t="s">
-        <v>986</v>
+        <v>997</v>
       </c>
       <c r="H164" s="0" t="s">
-        <v>987</v>
+        <v>998</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>988</v>
+        <v>999</v>
       </c>
       <c r="K164" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M164" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q164" s="0" t="s">
+        <v>1000</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10311,7 +10434,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>989</v>
+        <v>1001</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>267</v>
@@ -10323,19 +10446,25 @@
         <v>236</v>
       </c>
       <c r="F165" s="12" t="s">
-        <v>990</v>
+        <v>1002</v>
       </c>
       <c r="H165" s="0" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
       <c r="K165" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M165" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q165" s="0" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10343,10 +10472,10 @@
         <v>164</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>993</v>
+        <v>1006</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>994</v>
+        <v>1007</v>
       </c>
       <c r="D166" s="0" t="n">
         <v>2019</v>
@@ -10355,22 +10484,25 @@
         <v>236</v>
       </c>
       <c r="F166" s="22" t="s">
-        <v>995</v>
+        <v>1008</v>
       </c>
       <c r="G166" s="0" t="s">
-        <v>996</v>
+        <v>1009</v>
       </c>
       <c r="H166" s="0" t="s">
-        <v>997</v>
+        <v>1010</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>998</v>
+        <v>1011</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M166" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O166" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10378,10 +10510,10 @@
         <v>165</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>999</v>
+        <v>1012</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>1000</v>
+        <v>1013</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>2016</v>
@@ -10390,22 +10522,25 @@
         <v>236</v>
       </c>
       <c r="F167" s="22" t="s">
-        <v>1001</v>
+        <v>1014</v>
       </c>
       <c r="G167" s="0" t="s">
-        <v>1002</v>
+        <v>1015</v>
       </c>
       <c r="H167" s="0" t="s">
-        <v>1003</v>
+        <v>1016</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>1004</v>
+        <v>1017</v>
       </c>
       <c r="K167" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M167" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O167" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10413,10 +10548,10 @@
         <v>166</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>1005</v>
+        <v>1018</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>1006</v>
+        <v>1019</v>
       </c>
       <c r="D168" s="0" t="n">
         <v>2016</v>
@@ -10425,22 +10560,25 @@
         <v>236</v>
       </c>
       <c r="F168" s="12" t="s">
-        <v>1007</v>
+        <v>1020</v>
       </c>
       <c r="G168" s="0" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="H168" s="0" t="s">
-        <v>1009</v>
+        <v>1022</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>1010</v>
+        <v>1023</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M168" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O168" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10448,10 +10586,10 @@
         <v>167</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>1011</v>
+        <v>1024</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>1012</v>
+        <v>1025</v>
       </c>
       <c r="D169" s="0" t="n">
         <v>2016</v>
@@ -10460,22 +10598,28 @@
         <v>236</v>
       </c>
       <c r="F169" s="12" t="s">
-        <v>1013</v>
+        <v>1026</v>
       </c>
       <c r="G169" s="0" t="s">
-        <v>1014</v>
+        <v>1027</v>
       </c>
       <c r="H169" s="0" t="s">
-        <v>1015</v>
+        <v>1028</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>1016</v>
+        <v>1029</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M169" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q169" s="0" t="s">
+        <v>1030</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10483,10 +10627,10 @@
         <v>168</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>1017</v>
+        <v>1031</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>1018</v>
+        <v>1032</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>2019</v>
@@ -10495,22 +10639,25 @@
         <v>236</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>1019</v>
+        <v>1033</v>
       </c>
       <c r="G170" s="0" t="s">
-        <v>1020</v>
+        <v>1034</v>
       </c>
       <c r="H170" s="0" t="s">
-        <v>1021</v>
+        <v>1035</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>1022</v>
+        <v>1036</v>
       </c>
       <c r="K170" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M170" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O170" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10518,10 +10665,10 @@
         <v>169</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>1023</v>
+        <v>1037</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>1024</v>
+        <v>1038</v>
       </c>
       <c r="D171" s="0" t="n">
         <v>2019</v>
@@ -10530,22 +10677,28 @@
         <v>236</v>
       </c>
       <c r="F171" s="22" t="s">
-        <v>1025</v>
+        <v>1039</v>
       </c>
       <c r="G171" s="0" t="s">
-        <v>1026</v>
+        <v>1040</v>
       </c>
       <c r="H171" s="0" t="s">
-        <v>1027</v>
+        <v>1041</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>1028</v>
+        <v>1042</v>
       </c>
       <c r="K171" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M171" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="0" t="s">
+        <v>1043</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10553,10 +10706,10 @@
         <v>170</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>1029</v>
+        <v>1044</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>1030</v>
+        <v>1045</v>
       </c>
       <c r="D172" s="0" t="n">
         <v>2018</v>
@@ -10565,22 +10718,28 @@
         <v>236</v>
       </c>
       <c r="F172" s="12" t="s">
-        <v>1031</v>
+        <v>1046</v>
       </c>
       <c r="G172" s="0" t="s">
-        <v>1032</v>
+        <v>1047</v>
       </c>
       <c r="H172" s="0" t="s">
-        <v>1033</v>
+        <v>1048</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>1034</v>
+        <v>1049</v>
       </c>
       <c r="K172" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M172" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q172" s="0" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10588,10 +10747,10 @@
         <v>171</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>1035</v>
+        <v>1051</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>1036</v>
+        <v>1052</v>
       </c>
       <c r="D173" s="0" t="n">
         <v>2017</v>
@@ -10600,19 +10759,25 @@
         <v>236</v>
       </c>
       <c r="F173" s="12" t="s">
-        <v>1037</v>
+        <v>1053</v>
       </c>
       <c r="H173" s="0" t="s">
-        <v>1038</v>
+        <v>1054</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>1039</v>
+        <v>1055</v>
       </c>
       <c r="K173" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M173" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q173" s="0" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10620,10 +10785,10 @@
         <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>1040</v>
+        <v>1057</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>1041</v>
+        <v>1058</v>
       </c>
       <c r="D174" s="0" t="n">
         <v>2018</v>
@@ -10632,22 +10797,28 @@
         <v>236</v>
       </c>
       <c r="F174" s="12" t="s">
-        <v>1042</v>
+        <v>1059</v>
       </c>
       <c r="G174" s="0" t="s">
-        <v>1043</v>
+        <v>1060</v>
       </c>
       <c r="H174" s="0" t="s">
-        <v>1044</v>
+        <v>1061</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>1045</v>
+        <v>1062</v>
       </c>
       <c r="K174" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M174" s="0" t="s">
         <v>241</v>
+      </c>
+      <c r="O174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q174" s="0" t="s">
+        <v>1063</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10655,10 +10826,10 @@
         <v>173</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>1047</v>
+        <v>1065</v>
       </c>
       <c r="D175" s="0" t="n">
         <v>2018</v>
@@ -10667,16 +10838,16 @@
         <v>236</v>
       </c>
       <c r="F175" s="12" t="s">
-        <v>1048</v>
+        <v>1066</v>
       </c>
       <c r="G175" s="0" t="s">
-        <v>1049</v>
+        <v>1067</v>
       </c>
       <c r="H175" s="0" t="s">
-        <v>1050</v>
+        <v>1068</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>1051</v>
+        <v>1069</v>
       </c>
       <c r="K175" s="2" t="s">
         <v>63</v>
@@ -10690,7 +10861,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>1052</v>
+        <v>1070</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>357</v>
@@ -10702,16 +10873,16 @@
         <v>236</v>
       </c>
       <c r="F176" s="12" t="s">
-        <v>1053</v>
+        <v>1071</v>
       </c>
       <c r="G176" s="0" t="s">
-        <v>1054</v>
+        <v>1072</v>
       </c>
       <c r="H176" s="0" t="s">
-        <v>1055</v>
+        <v>1073</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>1056</v>
+        <v>1074</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>63</v>
@@ -10725,10 +10896,10 @@
         <v>175</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>1057</v>
+        <v>1075</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>1058</v>
+        <v>1076</v>
       </c>
       <c r="D177" s="0" t="n">
         <v>2018</v>
@@ -10737,16 +10908,16 @@
         <v>236</v>
       </c>
       <c r="F177" s="12" t="s">
-        <v>1059</v>
+        <v>1077</v>
       </c>
       <c r="G177" s="0" t="s">
-        <v>1060</v>
+        <v>1078</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>1061</v>
+        <v>1079</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>1062</v>
+        <v>1080</v>
       </c>
       <c r="K177" s="2" t="s">
         <v>63</v>
@@ -10760,10 +10931,10 @@
         <v>176</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>1063</v>
+        <v>1081</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>1064</v>
+        <v>1082</v>
       </c>
       <c r="D178" s="0" t="n">
         <v>2017</v>
@@ -10772,16 +10943,16 @@
         <v>236</v>
       </c>
       <c r="F178" s="12" t="s">
-        <v>1065</v>
+        <v>1083</v>
       </c>
       <c r="G178" s="0" t="s">
-        <v>1066</v>
+        <v>1084</v>
       </c>
       <c r="H178" s="0" t="s">
-        <v>1067</v>
+        <v>1085</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>1068</v>
+        <v>1086</v>
       </c>
       <c r="K178" s="2" t="s">
         <v>63</v>
@@ -10795,10 +10966,10 @@
         <v>177</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>1069</v>
+        <v>1087</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>1070</v>
+        <v>1088</v>
       </c>
       <c r="D179" s="0" t="n">
         <v>2019</v>
@@ -10807,16 +10978,16 @@
         <v>236</v>
       </c>
       <c r="F179" s="22" t="s">
-        <v>1071</v>
+        <v>1089</v>
       </c>
       <c r="G179" s="0" t="s">
-        <v>1072</v>
+        <v>1090</v>
       </c>
       <c r="H179" s="0" t="s">
-        <v>1073</v>
+        <v>1091</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>1074</v>
+        <v>1092</v>
       </c>
       <c r="K179" s="2" t="s">
         <v>63</v>
@@ -10830,10 +11001,10 @@
         <v>178</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>1075</v>
+        <v>1093</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1030</v>
+        <v>1045</v>
       </c>
       <c r="D180" s="0" t="n">
         <v>2018</v>
@@ -10842,16 +11013,16 @@
         <v>236</v>
       </c>
       <c r="F180" s="12" t="s">
-        <v>1076</v>
+        <v>1094</v>
       </c>
       <c r="G180" s="0" t="s">
-        <v>1077</v>
+        <v>1095</v>
       </c>
       <c r="H180" s="0" t="s">
-        <v>1078</v>
+        <v>1096</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>1079</v>
+        <v>1097</v>
       </c>
       <c r="K180" s="2" t="s">
         <v>63</v>
@@ -10865,10 +11036,10 @@
         <v>179</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>1080</v>
+        <v>1098</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>1030</v>
+        <v>1045</v>
       </c>
       <c r="D181" s="0" t="n">
         <v>2018</v>
@@ -10877,16 +11048,16 @@
         <v>236</v>
       </c>
       <c r="F181" s="12" t="s">
-        <v>1081</v>
+        <v>1099</v>
       </c>
       <c r="G181" s="0" t="s">
-        <v>1082</v>
+        <v>1100</v>
       </c>
       <c r="H181" s="0" t="s">
-        <v>1083</v>
+        <v>1101</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>1084</v>
+        <v>1102</v>
       </c>
       <c r="K181" s="2" t="s">
         <v>63</v>
@@ -10900,10 +11071,10 @@
         <v>180</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>1085</v>
+        <v>1103</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1086</v>
+        <v>1104</v>
       </c>
       <c r="D182" s="0" t="n">
         <v>2017</v>
@@ -10912,13 +11083,13 @@
         <v>236</v>
       </c>
       <c r="F182" s="12" t="s">
-        <v>1087</v>
+        <v>1105</v>
       </c>
       <c r="H182" s="0" t="s">
-        <v>1088</v>
+        <v>1106</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>1089</v>
+        <v>1107</v>
       </c>
       <c r="K182" s="2" t="s">
         <v>63</v>
@@ -10932,7 +11103,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>1090</v>
+        <v>1108</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>267</v>
@@ -10944,13 +11115,13 @@
         <v>236</v>
       </c>
       <c r="F183" s="12" t="s">
-        <v>1091</v>
+        <v>1109</v>
       </c>
       <c r="H183" s="0" t="s">
-        <v>1092</v>
+        <v>1110</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>1093</v>
+        <v>1111</v>
       </c>
       <c r="K183" s="2" t="s">
         <v>63</v>
@@ -10964,10 +11135,10 @@
         <v>182</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>1094</v>
+        <v>1112</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>1095</v>
+        <v>1113</v>
       </c>
       <c r="D184" s="0" t="n">
         <v>2017</v>
@@ -10976,13 +11147,13 @@
         <v>236</v>
       </c>
       <c r="F184" s="12" t="s">
-        <v>1096</v>
+        <v>1114</v>
       </c>
       <c r="H184" s="0" t="s">
-        <v>1097</v>
+        <v>1115</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>1098</v>
+        <v>1116</v>
       </c>
       <c r="K184" s="2" t="s">
         <v>63</v>
@@ -10996,10 +11167,10 @@
         <v>183</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>1099</v>
+        <v>1117</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>1100</v>
+        <v>1118</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>2018</v>
@@ -11008,16 +11179,16 @@
         <v>236</v>
       </c>
       <c r="F185" s="22" t="s">
-        <v>1101</v>
+        <v>1119</v>
       </c>
       <c r="G185" s="0" t="s">
-        <v>1102</v>
+        <v>1120</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>1103</v>
+        <v>1121</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>1104</v>
+        <v>1122</v>
       </c>
       <c r="K185" s="2" t="s">
         <v>63</v>
@@ -11031,10 +11202,10 @@
         <v>184</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>1105</v>
+        <v>1123</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>1106</v>
+        <v>1124</v>
       </c>
       <c r="D186" s="0" t="n">
         <v>2016</v>
@@ -11043,16 +11214,16 @@
         <v>236</v>
       </c>
       <c r="F186" s="12" t="s">
-        <v>1107</v>
+        <v>1125</v>
       </c>
       <c r="G186" s="0" t="s">
-        <v>1108</v>
+        <v>1126</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>1109</v>
+        <v>1127</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>1110</v>
+        <v>1128</v>
       </c>
       <c r="K186" s="2" t="s">
         <v>63</v>
@@ -11066,10 +11237,10 @@
         <v>185</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>1111</v>
+        <v>1129</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>1112</v>
+        <v>1130</v>
       </c>
       <c r="D187" s="0" t="n">
         <v>2016</v>
@@ -11078,13 +11249,13 @@
         <v>236</v>
       </c>
       <c r="F187" s="12" t="s">
-        <v>1113</v>
+        <v>1131</v>
       </c>
       <c r="H187" s="0" t="s">
-        <v>1114</v>
+        <v>1132</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>1115</v>
+        <v>1133</v>
       </c>
       <c r="K187" s="2" t="s">
         <v>63</v>
@@ -11098,10 +11269,10 @@
         <v>186</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>1116</v>
+        <v>1134</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>1117</v>
+        <v>1135</v>
       </c>
       <c r="D188" s="0" t="n">
         <v>2016</v>
@@ -11110,16 +11281,16 @@
         <v>236</v>
       </c>
       <c r="F188" s="12" t="s">
-        <v>1118</v>
+        <v>1136</v>
       </c>
       <c r="G188" s="0" t="s">
-        <v>1119</v>
+        <v>1137</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>1120</v>
+        <v>1138</v>
       </c>
       <c r="I188" s="2" t="s">
-        <v>1121</v>
+        <v>1139</v>
       </c>
       <c r="K188" s="2" t="s">
         <v>63</v>
@@ -11133,10 +11304,10 @@
         <v>187</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>1122</v>
+        <v>1140</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>1123</v>
+        <v>1141</v>
       </c>
       <c r="D189" s="0" t="n">
         <v>2016</v>
@@ -11145,16 +11316,16 @@
         <v>236</v>
       </c>
       <c r="F189" s="12" t="s">
-        <v>1124</v>
+        <v>1142</v>
       </c>
       <c r="G189" s="0" t="s">
-        <v>1125</v>
+        <v>1143</v>
       </c>
       <c r="H189" s="0" t="s">
-        <v>1126</v>
+        <v>1144</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>1127</v>
+        <v>1145</v>
       </c>
       <c r="K189" s="2" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Continue inclusion phase 2
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -4068,8 +4068,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C70" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q90" activeCellId="0" sqref="Q90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D102" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N105" activeCellId="0" sqref="N105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8371,6 +8371,15 @@
       <c r="O90" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P90" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R90" s="33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="n">
@@ -8409,6 +8418,15 @@
       <c r="O91" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P91" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q91" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="n">
@@ -8447,6 +8465,15 @@
       <c r="O92" s="31" t="n">
         <v>2</v>
       </c>
+      <c r="P92" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="13" t="n">
@@ -8485,6 +8512,15 @@
       <c r="O93" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P93" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R93" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="13" t="n">
@@ -8523,6 +8559,15 @@
       <c r="O94" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P94" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R94" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="13" t="n">
@@ -8602,6 +8647,15 @@
       <c r="O96" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P96" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R96" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="13" t="n">
@@ -8722,6 +8776,15 @@
       <c r="O99" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P99" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R99" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="n">
@@ -8760,6 +8823,15 @@
       <c r="O100" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P100" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R100" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="13" t="n">
@@ -8798,6 +8870,15 @@
       <c r="O101" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P101" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R101" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="n">
@@ -8833,6 +8914,15 @@
       <c r="O102" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P102" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R102" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="n">
@@ -8871,6 +8961,15 @@
       <c r="O103" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P103" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q103" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R103" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="n">
@@ -8950,6 +9049,15 @@
       <c r="O105" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P105" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R105" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="13" t="n">
@@ -8988,6 +9096,15 @@
       <c r="O106" s="31" t="n">
         <v>1</v>
       </c>
+      <c r="P106" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R106" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="13" t="n">
@@ -9024,6 +9141,15 @@
         <v>253</v>
       </c>
       <c r="O107" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="P107" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R107" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12257,7 +12383,7 @@
       </c>
       <c r="R190" s="40" t="n">
         <f aca="false">COUNTIFS(R3:R189, "=1")</f>
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="S190" s="43"/>
       <c r="AMJ190" s="0"/>

</xml_diff>

<commit_message>
Separate accepted paper to different sheet
- Update process description
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843BEA8-2225-4DBC-9AAA-D20946BA0D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFC949-CDDD-4FA1-9866-EB3930DCB3CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29055" yWindow="165" windowWidth="48675" windowHeight="15375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Initial Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Accepted Papers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="1188">
   <si>
     <t>Material search results</t>
   </si>
@@ -3596,6 +3597,9 @@
   </si>
   <si>
     <t>Animats, Q-learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papers accepted for mapping </t>
   </si>
 </sst>
 </file>
@@ -4314,8 +4318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4325,6 +4329,7 @@
     <col min="3" max="3" width="40.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="38.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" style="2" customWidth="1"/>
@@ -13067,4 +13072,3406 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B71EA-290D-4309-8558-374C60EDEE62}">
+  <dimension ref="A1:AME97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" style="1" customWidth="1"/>
+    <col min="2" max="2" width="111.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="46.42578125" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1019" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1019" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AME2"/>
+    </row>
+    <row r="3" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="2">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="2">
+        <v>8</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="2">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2016</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="2">
+        <v>78</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N12" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N14" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N15" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N16" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17">
+        <v>2019</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="G17" t="s">
+        <v>252</v>
+      </c>
+      <c r="H17" t="s">
+        <v>253</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18">
+        <v>2015</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="G18" t="s">
+        <v>259</v>
+      </c>
+      <c r="H18" t="s">
+        <v>260</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="16">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D19">
+        <v>2015</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" t="s">
+        <v>265</v>
+      </c>
+      <c r="H19" t="s">
+        <v>266</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D20">
+        <v>2018</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="G20" t="s">
+        <v>271</v>
+      </c>
+      <c r="H20" t="s">
+        <v>272</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21">
+        <v>2015</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="G21" t="s">
+        <v>277</v>
+      </c>
+      <c r="H21" t="s">
+        <v>278</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22">
+        <v>2018</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="G22" t="s">
+        <v>283</v>
+      </c>
+      <c r="H22" t="s">
+        <v>284</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D23">
+        <v>2016</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="G23" t="s">
+        <v>289</v>
+      </c>
+      <c r="H23" t="s">
+        <v>290</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D24">
+        <v>2015</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="G24" t="s">
+        <v>295</v>
+      </c>
+      <c r="H24" t="s">
+        <v>296</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="16">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D25">
+        <v>2017</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="G25" t="s">
+        <v>301</v>
+      </c>
+      <c r="H25" t="s">
+        <v>302</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <v>45</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26">
+        <v>2019</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="H26" t="s">
+        <v>307</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D27">
+        <v>2017</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" t="s">
+        <v>312</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D28">
+        <v>2018</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="G28" t="s">
+        <v>317</v>
+      </c>
+      <c r="H28" t="s">
+        <v>318</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>48</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D29">
+        <v>2017</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="G29" t="s">
+        <v>323</v>
+      </c>
+      <c r="H29" t="s">
+        <v>324</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="16">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30">
+        <v>2016</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="H30" t="s">
+        <v>329</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
+        <v>50</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D31">
+        <v>2019</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="G31" t="s">
+        <v>333</v>
+      </c>
+      <c r="H31" t="s">
+        <v>334</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="16">
+        <v>51</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32">
+        <v>2015</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="G32" t="s">
+        <v>338</v>
+      </c>
+      <c r="H32" t="s">
+        <v>339</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="16">
+        <v>52</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D33">
+        <v>2017</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="G33" t="s">
+        <v>344</v>
+      </c>
+      <c r="H33" t="s">
+        <v>345</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="16">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D34">
+        <v>2015</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="G34" t="s">
+        <v>356</v>
+      </c>
+      <c r="H34" t="s">
+        <v>357</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="16">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D35">
+        <v>2019</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="G35" t="s">
+        <v>362</v>
+      </c>
+      <c r="H35" t="s">
+        <v>363</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="16">
+        <v>56</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D36">
+        <v>2018</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="G36" t="s">
+        <v>368</v>
+      </c>
+      <c r="H36" t="s">
+        <v>369</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="16">
+        <v>57</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D37">
+        <v>2015</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="G37" t="s">
+        <v>374</v>
+      </c>
+      <c r="H37" t="s">
+        <v>375</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="16">
+        <v>58</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D38">
+        <v>2015</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="G38" t="s">
+        <v>380</v>
+      </c>
+      <c r="H38" t="s">
+        <v>381</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="16">
+        <v>59</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D39">
+        <v>2018</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="G39" t="s">
+        <v>386</v>
+      </c>
+      <c r="H39" t="s">
+        <v>387</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16">
+        <v>61</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D40">
+        <v>2017</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="H40" t="s">
+        <v>397</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="16">
+        <v>62</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D41">
+        <v>2016</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="G41" t="s">
+        <v>402</v>
+      </c>
+      <c r="H41" t="s">
+        <v>403</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="16">
+        <v>63</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D42">
+        <v>2019</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>407</v>
+      </c>
+      <c r="G42" t="s">
+        <v>408</v>
+      </c>
+      <c r="H42" t="s">
+        <v>409</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
+        <v>64</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D43">
+        <v>2016</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="G43" t="s">
+        <v>414</v>
+      </c>
+      <c r="H43" t="s">
+        <v>415</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="16">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D44">
+        <v>2018</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="G44" t="s">
+        <v>420</v>
+      </c>
+      <c r="H44" t="s">
+        <v>421</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M44" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="16">
+        <v>67</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D45">
+        <v>2015</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="G45" t="s">
+        <v>432</v>
+      </c>
+      <c r="H45" t="s">
+        <v>433</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="16">
+        <v>68</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D46">
+        <v>2019</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="G46" t="s">
+        <v>438</v>
+      </c>
+      <c r="H46" t="s">
+        <v>439</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M46" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="16">
+        <v>69</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D47">
+        <v>2018</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="H47" t="s">
+        <v>443</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
+        <v>71</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D48">
+        <v>2018</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="G48" t="s">
+        <v>454</v>
+      </c>
+      <c r="H48" t="s">
+        <v>455</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M48" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="16">
+        <v>72</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D49">
+        <v>2016</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="H49" t="s">
+        <v>460</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="16">
+        <v>73</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D50">
+        <v>2015</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="H50" t="s">
+        <v>465</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="16">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D51">
+        <v>2017</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>476</v>
+      </c>
+      <c r="G51" t="s">
+        <v>477</v>
+      </c>
+      <c r="H51" t="s">
+        <v>478</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="16">
+        <v>78</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D52">
+        <v>2016</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="G52" t="s">
+        <v>497</v>
+      </c>
+      <c r="H52" t="s">
+        <v>498</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="16">
+        <v>80</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D53">
+        <v>2018</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="G53" t="s">
+        <v>510</v>
+      </c>
+      <c r="H53" t="s">
+        <v>511</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M53" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="16">
+        <v>81</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="D54">
+        <v>2017</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="H54" t="s">
+        <v>516</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="16">
+        <v>82</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D55">
+        <v>2016</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="G55" t="s">
+        <v>521</v>
+      </c>
+      <c r="H55" t="s">
+        <v>522</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="16">
+        <v>85</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="D56">
+        <v>2015</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="G56" t="s">
+        <v>540</v>
+      </c>
+      <c r="H56" t="s">
+        <v>541</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="16">
+        <v>86</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D57">
+        <v>2016</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>545</v>
+      </c>
+      <c r="G57" t="s">
+        <v>546</v>
+      </c>
+      <c r="H57" t="s">
+        <v>547</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="16">
+        <v>87</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D58">
+        <v>2018</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="G58" t="s">
+        <v>552</v>
+      </c>
+      <c r="H58" t="s">
+        <v>553</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="16">
+        <v>88</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D59">
+        <v>2015</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="G59" t="s">
+        <v>558</v>
+      </c>
+      <c r="H59" t="s">
+        <v>559</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M59" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="16">
+        <v>89</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60">
+        <v>2015</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>562</v>
+      </c>
+      <c r="G60" t="s">
+        <v>563</v>
+      </c>
+      <c r="H60" t="s">
+        <v>564</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M60" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="16">
+        <v>90</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D61">
+        <v>2016</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>568</v>
+      </c>
+      <c r="G61" t="s">
+        <v>569</v>
+      </c>
+      <c r="H61" t="s">
+        <v>570</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="16">
+        <v>91</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62">
+        <v>2018</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>573</v>
+      </c>
+      <c r="G62" t="s">
+        <v>574</v>
+      </c>
+      <c r="H62" t="s">
+        <v>575</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M62" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="16">
+        <v>92</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D63">
+        <v>2019</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>579</v>
+      </c>
+      <c r="G63" t="s">
+        <v>580</v>
+      </c>
+      <c r="H63" t="s">
+        <v>581</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M63" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="16">
+        <v>94</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D64">
+        <v>2016</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="G64" t="s">
+        <v>593</v>
+      </c>
+      <c r="H64" t="s">
+        <v>594</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M64" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="16">
+        <v>97</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D65">
+        <v>2019</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F65" s="36" t="s">
+        <v>612</v>
+      </c>
+      <c r="G65" t="s">
+        <v>613</v>
+      </c>
+      <c r="H65" t="s">
+        <v>614</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M65" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="16">
+        <v>98</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D66">
+        <v>2018</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>618</v>
+      </c>
+      <c r="G66" t="s">
+        <v>619</v>
+      </c>
+      <c r="H66" t="s">
+        <v>620</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M66" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="16">
+        <v>99</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="D67">
+        <v>2018</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="G67" t="s">
+        <v>625</v>
+      </c>
+      <c r="H67" t="s">
+        <v>626</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M67" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="16">
+        <v>100</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D68">
+        <v>2017</v>
+      </c>
+      <c r="E68" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>629</v>
+      </c>
+      <c r="H68" t="s">
+        <v>630</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="16">
+        <v>101</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D69">
+        <v>2018</v>
+      </c>
+      <c r="E69" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F69" s="18" t="s">
+        <v>634</v>
+      </c>
+      <c r="G69" t="s">
+        <v>635</v>
+      </c>
+      <c r="H69" t="s">
+        <v>636</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M69" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="16">
+        <v>103</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="D70">
+        <v>2016</v>
+      </c>
+      <c r="E70" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>647</v>
+      </c>
+      <c r="G70" t="s">
+        <v>648</v>
+      </c>
+      <c r="H70" t="s">
+        <v>649</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="16">
+        <v>104</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="D71">
+        <v>2016</v>
+      </c>
+      <c r="E71" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F71" s="18" t="s">
+        <v>653</v>
+      </c>
+      <c r="G71" t="s">
+        <v>654</v>
+      </c>
+      <c r="H71" t="s">
+        <v>655</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M71" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="16">
+        <v>105</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D72">
+        <v>2016</v>
+      </c>
+      <c r="E72" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F72" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="G72" t="s">
+        <v>660</v>
+      </c>
+      <c r="H72" t="s">
+        <v>661</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M72" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="16">
+        <v>106</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="D73">
+        <v>2016</v>
+      </c>
+      <c r="E73" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="G73" t="s">
+        <v>666</v>
+      </c>
+      <c r="H73" t="s">
+        <v>667</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="16">
+        <v>107</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74">
+        <v>2016</v>
+      </c>
+      <c r="E74" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>670</v>
+      </c>
+      <c r="G74" t="s">
+        <v>671</v>
+      </c>
+      <c r="H74" t="s">
+        <v>672</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M74" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="16">
+        <v>112</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="D75">
+        <v>2018</v>
+      </c>
+      <c r="E75" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F75" s="36" t="s">
+        <v>703</v>
+      </c>
+      <c r="G75" t="s">
+        <v>704</v>
+      </c>
+      <c r="H75" t="s">
+        <v>705</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M75" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="16">
+        <v>114</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="D76">
+        <v>2016</v>
+      </c>
+      <c r="E76" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>716</v>
+      </c>
+      <c r="G76" t="s">
+        <v>717</v>
+      </c>
+      <c r="H76" t="s">
+        <v>718</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M76" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="16">
+        <v>115</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="D77">
+        <v>2016</v>
+      </c>
+      <c r="E77" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>722</v>
+      </c>
+      <c r="G77" t="s">
+        <v>723</v>
+      </c>
+      <c r="H77" t="s">
+        <v>724</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M77" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="16">
+        <v>117</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="D78">
+        <v>2019</v>
+      </c>
+      <c r="E78" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F78" s="36" t="s">
+        <v>735</v>
+      </c>
+      <c r="G78" t="s">
+        <v>736</v>
+      </c>
+      <c r="H78" t="s">
+        <v>737</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M78" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="16">
+        <v>118</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="D79">
+        <v>2017</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>741</v>
+      </c>
+      <c r="H79" t="s">
+        <v>742</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="16">
+        <v>121</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="D80">
+        <v>2017</v>
+      </c>
+      <c r="E80" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F80" s="36" t="s">
+        <v>760</v>
+      </c>
+      <c r="H80" t="s">
+        <v>761</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="16">
+        <v>124</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D81">
+        <v>2017</v>
+      </c>
+      <c r="E81" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F81" s="18" t="s">
+        <v>779</v>
+      </c>
+      <c r="G81" t="s">
+        <v>780</v>
+      </c>
+      <c r="H81" t="s">
+        <v>781</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M81" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="16">
+        <v>127</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="D82">
+        <v>2018</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F82" s="18" t="s">
+        <v>799</v>
+      </c>
+      <c r="G82" t="s">
+        <v>800</v>
+      </c>
+      <c r="H82" t="s">
+        <v>801</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="16">
+        <v>128</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="D83">
+        <v>2015</v>
+      </c>
+      <c r="E83" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>805</v>
+      </c>
+      <c r="G83" t="s">
+        <v>806</v>
+      </c>
+      <c r="H83" t="s">
+        <v>807</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M83" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16">
+        <v>131</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="D84">
+        <v>2015</v>
+      </c>
+      <c r="E84" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F84" s="18" t="s">
+        <v>825</v>
+      </c>
+      <c r="G84" t="s">
+        <v>826</v>
+      </c>
+      <c r="H84" t="s">
+        <v>827</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M84" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="16">
+        <v>132</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="D85">
+        <v>2017</v>
+      </c>
+      <c r="E85" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>831</v>
+      </c>
+      <c r="H85" t="s">
+        <v>832</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="16">
+        <v>134</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="D86">
+        <v>2018</v>
+      </c>
+      <c r="E86" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F86" s="36" t="s">
+        <v>842</v>
+      </c>
+      <c r="G86" t="s">
+        <v>766</v>
+      </c>
+      <c r="H86" t="s">
+        <v>843</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M86" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="16">
+        <v>138</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="D87">
+        <v>2016</v>
+      </c>
+      <c r="E87" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F87" s="36" t="s">
+        <v>868</v>
+      </c>
+      <c r="G87" t="s">
+        <v>869</v>
+      </c>
+      <c r="H87" t="s">
+        <v>870</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="16">
+        <v>139</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D88">
+        <v>2019</v>
+      </c>
+      <c r="E88" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F88" s="36" t="s">
+        <v>874</v>
+      </c>
+      <c r="G88" t="s">
+        <v>875</v>
+      </c>
+      <c r="H88" t="s">
+        <v>876</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M88" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="16">
+        <v>141</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D89">
+        <v>2018</v>
+      </c>
+      <c r="E89" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>885</v>
+      </c>
+      <c r="G89" t="s">
+        <v>886</v>
+      </c>
+      <c r="H89" t="s">
+        <v>887</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M89" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="16">
+        <v>144</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="D90">
+        <v>2018</v>
+      </c>
+      <c r="E90" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>904</v>
+      </c>
+      <c r="G90" t="s">
+        <v>905</v>
+      </c>
+      <c r="H90" t="s">
+        <v>906</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M90" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="16">
+        <v>145</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D91">
+        <v>2016</v>
+      </c>
+      <c r="E91" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F91" s="18" t="s">
+        <v>910</v>
+      </c>
+      <c r="H91" t="s">
+        <v>911</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M91" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="16">
+        <v>147</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D92">
+        <v>2016</v>
+      </c>
+      <c r="E92" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F92" s="18" t="s">
+        <v>920</v>
+      </c>
+      <c r="G92" t="s">
+        <v>921</v>
+      </c>
+      <c r="H92" t="s">
+        <v>922</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M92" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="16">
+        <v>164</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D93">
+        <v>2019</v>
+      </c>
+      <c r="E93" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F93" s="36" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G93" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H93" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M93" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="16">
+        <v>174</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D94">
+        <v>2017</v>
+      </c>
+      <c r="E94" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F94" s="18" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G94" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H94" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M94" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1019" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16">
+        <v>185</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D95">
+        <v>2016</v>
+      </c>
+      <c r="E95" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F95" s="18" t="s">
+        <v>1167</v>
+      </c>
+      <c r="H95" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>1169</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M95" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1019" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="47">
+        <f>COUNT(A3:A95)</f>
+        <v>93</v>
+      </c>
+      <c r="B96" s="48"/>
+      <c r="C96" s="48"/>
+      <c r="E96" s="50"/>
+      <c r="F96" s="51"/>
+      <c r="I96" s="48"/>
+      <c r="J96" s="48"/>
+      <c r="K96" s="48"/>
+      <c r="AME96"/>
+    </row>
+    <row r="97" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E10:E97" xr:uid="{241F5E68-5F12-465A-A28D-BA53E5118789}">
+      <formula1>"JAGI,AIJ,JAIR,ICAGI,IJCAI,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Describe search, Prepare for keywording
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258E3B63-165C-434F-AFD0-CC348AC6097F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BA1D90-46AB-4DB3-A853-72F2DC726867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="1203">
   <si>
     <t>Material search results</t>
   </si>
@@ -3600,13 +3600,58 @@
   </si>
   <si>
     <t xml:space="preserve">Papers accepted for mapping </t>
+  </si>
+  <si>
+    <t>Search Summary</t>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>Total papers</t>
+  </si>
+  <si>
+    <t>Summa</t>
+  </si>
+  <si>
+    <t>Keskiarvo</t>
+  </si>
+  <si>
+    <t>Juokseva summa</t>
+  </si>
+  <si>
+    <t>Laske</t>
+  </si>
+  <si>
+    <t>Search Engine</t>
+  </si>
+  <si>
+    <t>Additional Limitations</t>
+  </si>
+  <si>
+    <t>Cognitive architecture</t>
+  </si>
+  <si>
+    <t>Accepted (%)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>JYU</t>
+  </si>
+  <si>
+    <t>Wieringa-classification</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3668,6 +3713,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -3750,7 +3801,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3796,8 +3847,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -3824,8 +3884,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -3920,8 +3981,15 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="19"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="5" xfId="26" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="27">
     <cellStyle name="Accent 1 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Bad" xfId="25" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
     <cellStyle name="Bad 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -3948,6 +4016,7 @@
     <cellStyle name="Neutral 7" xfId="22" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Neutral 8" xfId="23" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Prosenttia" xfId="26" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4327,10 +4396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ191"/>
+  <dimension ref="A1:AMJ200"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9727,6 +9796,9 @@
       <c r="R113" s="8">
         <v>0</v>
       </c>
+      <c r="S113" s="5" t="s">
+        <v>1197</v>
+      </c>
     </row>
     <row r="114" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="16">
@@ -13043,7 +13115,10 @@
       </c>
     </row>
     <row r="190" spans="1:1024" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="47"/>
+      <c r="A190" s="47">
+        <f>COUNT(A3:A189)</f>
+        <v>187</v>
+      </c>
       <c r="B190" s="48"/>
       <c r="C190" s="48"/>
       <c r="E190" s="50"/>
@@ -13069,15 +13144,184 @@
     <row r="191" spans="1:1024" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="16"/>
     </row>
+    <row r="193" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B193" s="58" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B194" s="60" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C194" s="60" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D194" s="61" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E194" s="60" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F194" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G194" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="H194" s="61" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B195" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E195" s="2">
+        <f>COUNTIF(E3:E189,"=JAIR")</f>
+        <v>5</v>
+      </c>
+      <c r="F195">
+        <f>COUNTIFS(E3:E189,"JAIR",O3:O189,"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="G195">
+        <f>COUNTIFS(E3:E189,"JAIR",R3:R189,"&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="H195" s="59">
+        <f>G195/E195</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="196" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B196" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E196" s="2">
+        <f>COUNTIF(E3:E189,"=IJCAI")</f>
+        <v>12</v>
+      </c>
+      <c r="F196">
+        <f>COUNTIFS(E4:E190,"IJCAI",O4:O190,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="G196">
+        <f>COUNTIFS(E3:E189,"IJCAI",R3:R189,"&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="H196" s="59">
+        <f t="shared" ref="H196:H200" si="0">G196/E196</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B197" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E197" s="2">
+        <f>COUNTIF(E3:E189,"=AIJ")</f>
+        <v>3</v>
+      </c>
+      <c r="F197">
+        <f>COUNTIFS(E4:E190,"AIJ",O4:O190,"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="G197">
+        <f>COUNTIFS(E3:E189,"AIJ",R3:R189,"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="H197" s="59">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B198" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E198" s="2">
+        <f>COUNTIF(E3:E189,"=JAGI")</f>
+        <v>15</v>
+      </c>
+      <c r="F198">
+        <f>COUNTIFS(E4:E190,"JAGI",O4:O190,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="G198">
+        <f>COUNTIFS(E3:E189,"JAGI",R3:R189,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="H198" s="59">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B199" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E199" s="2">
+        <f>COUNTIF(E3:E189,"=ICAGI")</f>
+        <v>152</v>
+      </c>
+      <c r="F199">
+        <f>COUNTIFS(E4:E190,"ICAGI",O4:O190,"&gt;0")</f>
+        <v>99</v>
+      </c>
+      <c r="G199">
+        <f>COUNTIFS(E3:E189,"ICAGI",R3:R189,"&gt;0")</f>
+        <v>79</v>
+      </c>
+      <c r="H199" s="59">
+        <f t="shared" si="0"/>
+        <v>0.51973684210526316</v>
+      </c>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B200" s="62"/>
+      <c r="C200" s="62"/>
+      <c r="D200" s="63"/>
+      <c r="E200" s="62">
+        <f>SUM(E195:E199)</f>
+        <v>187</v>
+      </c>
+      <c r="F200" s="63">
+        <f>SUM(F195:F199)</f>
+        <v>122</v>
+      </c>
+      <c r="G200" s="63">
+        <f>SUM(G195:G199)</f>
+        <v>93</v>
+      </c>
+      <c r="H200" s="64">
+        <f t="shared" si="0"/>
+        <v>0.49732620320855614</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E23:E191" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E23:E191 B198:B199" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"JAGI,AIJ,JAIR,ICAGI,IJCAI,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -13087,10 +13331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B71EA-290D-4309-8558-374C60EDEE62}">
-  <dimension ref="A1:AME97"/>
+  <dimension ref="A1:AMB97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13102,23 +13346,21 @@
     <col min="6" max="6" width="11.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" style="53" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="46.42578125" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="46.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1019" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1016" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>1187</v>
       </c>
     </row>
-    <row r="2" spans="1:1019" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1016" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -13147,35 +13389,29 @@
         <v>11</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>16</v>
+      <c r="M2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>1201</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AME2"/>
-    </row>
-    <row r="3" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1202</v>
+      </c>
+      <c r="AMB2"/>
+    </row>
+    <row r="3" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -13203,20 +13439,17 @@
       <c r="I3" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="3">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>5</v>
       </c>
@@ -13244,23 +13477,17 @@
       <c r="I4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="2">
-        <v>23</v>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="3">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>6</v>
       </c>
@@ -13288,23 +13515,17 @@
       <c r="I5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="2">
-        <v>8</v>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>8</v>
       </c>
@@ -13332,23 +13553,17 @@
       <c r="I6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="2">
-        <v>25</v>
+      <c r="J6" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>14</v>
       </c>
@@ -13373,20 +13588,17 @@
       <c r="H7" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="J7" s="2">
-        <v>78</v>
+      <c r="J7" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>17</v>
       </c>
@@ -13411,20 +13623,17 @@
       <c r="I8" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="J8" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K8" s="2" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>19</v>
       </c>
@@ -13452,23 +13661,17 @@
       <c r="I9" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J9" s="2">
-        <v>5</v>
+      <c r="J9" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>157</v>
+        <v>34</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N9" s="3">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>23</v>
       </c>
@@ -13490,20 +13693,17 @@
       <c r="I10" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>24</v>
       </c>
@@ -13528,20 +13728,17 @@
       <c r="I11" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N11" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>25</v>
       </c>
@@ -13566,20 +13763,17 @@
       <c r="I12" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N12" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
         <v>26</v>
       </c>
@@ -13604,20 +13798,17 @@
       <c r="I13" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N13" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
         <v>27</v>
       </c>
@@ -13642,20 +13833,17 @@
       <c r="I14" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N14" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
         <v>28</v>
       </c>
@@ -13680,20 +13868,17 @@
       <c r="I15" s="2" t="s">
         <v>205</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K15" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N15" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <v>34</v>
       </c>
@@ -13718,20 +13903,17 @@
       <c r="I16" s="2" t="s">
         <v>241</v>
       </c>
+      <c r="J16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="N16" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>36</v>
       </c>
@@ -13759,14 +13941,17 @@
       <c r="I17" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <v>37</v>
       </c>
@@ -13794,14 +13979,17 @@
       <c r="I18" s="2" t="s">
         <v>261</v>
       </c>
+      <c r="J18" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
         <v>38</v>
       </c>
@@ -13829,14 +14017,17 @@
       <c r="I19" s="2" t="s">
         <v>267</v>
       </c>
+      <c r="J19" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
         <v>39</v>
       </c>
@@ -13864,14 +14055,17 @@
       <c r="I20" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="J20" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
         <v>40</v>
       </c>
@@ -13899,14 +14093,17 @@
       <c r="I21" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="J21" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <v>41</v>
       </c>
@@ -13934,14 +14131,17 @@
       <c r="I22" s="2" t="s">
         <v>285</v>
       </c>
+      <c r="J22" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M22" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
         <v>42</v>
       </c>
@@ -13969,14 +14169,17 @@
       <c r="I23" s="2" t="s">
         <v>291</v>
       </c>
+      <c r="J23" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M23" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
         <v>43</v>
       </c>
@@ -14004,14 +14207,17 @@
       <c r="I24" s="2" t="s">
         <v>297</v>
       </c>
+      <c r="J24" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <v>44</v>
       </c>
@@ -14039,14 +14245,17 @@
       <c r="I25" s="2" t="s">
         <v>303</v>
       </c>
+      <c r="J25" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
         <v>45</v>
       </c>
@@ -14071,14 +14280,17 @@
       <c r="I26" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="J26" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L26" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
         <v>46</v>
       </c>
@@ -14103,14 +14315,17 @@
       <c r="I27" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="J27" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M27" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <v>47</v>
       </c>
@@ -14138,14 +14353,17 @@
       <c r="I28" s="2" t="s">
         <v>319</v>
       </c>
+      <c r="J28" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K28" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16">
         <v>48</v>
       </c>
@@ -14173,14 +14391,17 @@
       <c r="I29" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="J29" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M29" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16">
         <v>49</v>
       </c>
@@ -14205,14 +14426,17 @@
       <c r="I30" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="J30" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M30" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <v>50</v>
       </c>
@@ -14240,14 +14464,17 @@
       <c r="I31" s="2" t="s">
         <v>335</v>
       </c>
+      <c r="J31" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M31" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16">
         <v>51</v>
       </c>
@@ -14275,14 +14502,17 @@
       <c r="I32" s="2" t="s">
         <v>340</v>
       </c>
+      <c r="J32" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M32" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16">
         <v>52</v>
       </c>
@@ -14310,14 +14540,17 @@
       <c r="I33" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="J33" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M33" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16">
         <v>54</v>
       </c>
@@ -14345,14 +14578,17 @@
       <c r="I34" s="2" t="s">
         <v>358</v>
       </c>
+      <c r="J34" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
         <v>55</v>
       </c>
@@ -14380,14 +14616,17 @@
       <c r="I35" s="2" t="s">
         <v>364</v>
       </c>
+      <c r="J35" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16">
         <v>56</v>
       </c>
@@ -14415,14 +14654,17 @@
       <c r="I36" s="2" t="s">
         <v>370</v>
       </c>
+      <c r="J36" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K36" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M36" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>57</v>
       </c>
@@ -14450,14 +14692,17 @@
       <c r="I37" s="2" t="s">
         <v>376</v>
       </c>
+      <c r="J37" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="16">
         <v>58</v>
       </c>
@@ -14485,14 +14730,17 @@
       <c r="I38" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="J38" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M38" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16">
         <v>59</v>
       </c>
@@ -14520,14 +14768,17 @@
       <c r="I39" s="2" t="s">
         <v>388</v>
       </c>
+      <c r="J39" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M39" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="16">
         <v>61</v>
       </c>
@@ -14552,14 +14803,17 @@
       <c r="I40" s="2" t="s">
         <v>398</v>
       </c>
+      <c r="J40" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M40" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>62</v>
       </c>
@@ -14587,14 +14841,17 @@
       <c r="I41" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="J41" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M41" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16">
         <v>63</v>
       </c>
@@ -14622,14 +14879,17 @@
       <c r="I42" s="2" t="s">
         <v>410</v>
       </c>
+      <c r="J42" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M42" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16">
         <v>64</v>
       </c>
@@ -14657,14 +14917,17 @@
       <c r="I43" s="2" t="s">
         <v>416</v>
       </c>
+      <c r="J43" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M43" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16">
         <v>65</v>
       </c>
@@ -14692,14 +14955,17 @@
       <c r="I44" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="J44" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M44" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L44" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16">
         <v>67</v>
       </c>
@@ -14727,14 +14993,17 @@
       <c r="I45" s="2" t="s">
         <v>434</v>
       </c>
+      <c r="J45" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K45" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M45" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16">
         <v>68</v>
       </c>
@@ -14762,14 +15031,17 @@
       <c r="I46" s="2" t="s">
         <v>440</v>
       </c>
+      <c r="J46" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K46" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M46" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L46" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16">
         <v>69</v>
       </c>
@@ -14794,14 +15066,17 @@
       <c r="I47" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="J47" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K47" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M47" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16">
         <v>71</v>
       </c>
@@ -14829,14 +15104,17 @@
       <c r="I48" s="2" t="s">
         <v>456</v>
       </c>
+      <c r="J48" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K48" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M48" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L48" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16">
         <v>72</v>
       </c>
@@ -14861,14 +15139,17 @@
       <c r="I49" s="2" t="s">
         <v>461</v>
       </c>
+      <c r="J49" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K49" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M49" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="16">
         <v>73</v>
       </c>
@@ -14893,14 +15174,17 @@
       <c r="I50" s="2" t="s">
         <v>466</v>
       </c>
+      <c r="J50" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K50" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M50" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="16">
         <v>75</v>
       </c>
@@ -14928,14 +15212,17 @@
       <c r="I51" s="2" t="s">
         <v>479</v>
       </c>
+      <c r="J51" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K51" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M51" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="16">
         <v>78</v>
       </c>
@@ -14963,14 +15250,17 @@
       <c r="I52" s="2" t="s">
         <v>499</v>
       </c>
+      <c r="J52" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M52" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="16">
         <v>80</v>
       </c>
@@ -14998,14 +15288,17 @@
       <c r="I53" s="2" t="s">
         <v>512</v>
       </c>
+      <c r="J53" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K53" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M53" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L53" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16">
         <v>81</v>
       </c>
@@ -15030,14 +15323,17 @@
       <c r="I54" s="2" t="s">
         <v>517</v>
       </c>
+      <c r="J54" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M54" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="16">
         <v>82</v>
       </c>
@@ -15065,14 +15361,17 @@
       <c r="I55" s="2" t="s">
         <v>523</v>
       </c>
+      <c r="J55" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K55" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16">
         <v>85</v>
       </c>
@@ -15100,14 +15399,17 @@
       <c r="I56" s="2" t="s">
         <v>542</v>
       </c>
+      <c r="J56" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K56" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M56" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="16">
         <v>86</v>
       </c>
@@ -15135,14 +15437,17 @@
       <c r="I57" s="2" t="s">
         <v>548</v>
       </c>
+      <c r="J57" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K57" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M57" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16">
         <v>87</v>
       </c>
@@ -15170,14 +15475,17 @@
       <c r="I58" s="2" t="s">
         <v>554</v>
       </c>
+      <c r="J58" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K58" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M58" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="16">
         <v>88</v>
       </c>
@@ -15205,14 +15513,17 @@
       <c r="I59" s="2" t="s">
         <v>560</v>
       </c>
+      <c r="J59" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K59" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L59" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="16">
         <v>89</v>
       </c>
@@ -15240,14 +15551,17 @@
       <c r="I60" s="2" t="s">
         <v>565</v>
       </c>
+      <c r="J60" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K60" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M60" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L60" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="16">
         <v>90</v>
       </c>
@@ -15275,14 +15589,17 @@
       <c r="I61" s="2" t="s">
         <v>571</v>
       </c>
+      <c r="J61" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K61" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M61" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="16">
         <v>91</v>
       </c>
@@ -15310,14 +15627,17 @@
       <c r="I62" s="2" t="s">
         <v>576</v>
       </c>
+      <c r="J62" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K62" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M62" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L62" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="16">
         <v>92</v>
       </c>
@@ -15345,14 +15665,17 @@
       <c r="I63" s="2" t="s">
         <v>582</v>
       </c>
+      <c r="J63" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K63" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M63" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L63" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="16">
         <v>94</v>
       </c>
@@ -15380,14 +15703,17 @@
       <c r="I64" s="2" t="s">
         <v>595</v>
       </c>
+      <c r="J64" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M64" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L64" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16">
         <v>97</v>
       </c>
@@ -15415,14 +15741,17 @@
       <c r="I65" s="2" t="s">
         <v>615</v>
       </c>
+      <c r="J65" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K65" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M65" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L65" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="16">
         <v>98</v>
       </c>
@@ -15450,14 +15779,17 @@
       <c r="I66" s="2" t="s">
         <v>621</v>
       </c>
+      <c r="J66" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K66" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L66" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16">
         <v>99</v>
       </c>
@@ -15485,14 +15817,17 @@
       <c r="I67" s="2" t="s">
         <v>627</v>
       </c>
+      <c r="J67" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K67" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L67" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="16">
         <v>100</v>
       </c>
@@ -15517,14 +15852,17 @@
       <c r="I68" s="2" t="s">
         <v>631</v>
       </c>
+      <c r="J68" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K68" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16">
         <v>101</v>
       </c>
@@ -15552,14 +15890,17 @@
       <c r="I69" s="2" t="s">
         <v>637</v>
       </c>
+      <c r="J69" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K69" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M69" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L69" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16">
         <v>103</v>
       </c>
@@ -15587,14 +15928,17 @@
       <c r="I70" s="2" t="s">
         <v>650</v>
       </c>
+      <c r="J70" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K70" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M70" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16">
         <v>104</v>
       </c>
@@ -15622,14 +15966,17 @@
       <c r="I71" s="2" t="s">
         <v>656</v>
       </c>
+      <c r="J71" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M71" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L71" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16">
         <v>105</v>
       </c>
@@ -15657,14 +16004,17 @@
       <c r="I72" s="2" t="s">
         <v>662</v>
       </c>
+      <c r="J72" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K72" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M72" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L72" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16">
         <v>106</v>
       </c>
@@ -15692,14 +16042,17 @@
       <c r="I73" s="2" t="s">
         <v>668</v>
       </c>
+      <c r="J73" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K73" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M73" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16">
         <v>107</v>
       </c>
@@ -15727,14 +16080,17 @@
       <c r="I74" s="2" t="s">
         <v>673</v>
       </c>
+      <c r="J74" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K74" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M74" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L74" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16">
         <v>112</v>
       </c>
@@ -15762,14 +16118,17 @@
       <c r="I75" s="2" t="s">
         <v>706</v>
       </c>
+      <c r="J75" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K75" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M75" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L75" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16">
         <v>114</v>
       </c>
@@ -15797,14 +16156,17 @@
       <c r="I76" s="2" t="s">
         <v>719</v>
       </c>
+      <c r="J76" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K76" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M76" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L76" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16">
         <v>115</v>
       </c>
@@ -15832,14 +16194,17 @@
       <c r="I77" s="2" t="s">
         <v>725</v>
       </c>
+      <c r="J77" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K77" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M77" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L77" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16">
         <v>117</v>
       </c>
@@ -15867,14 +16232,17 @@
       <c r="I78" s="2" t="s">
         <v>738</v>
       </c>
+      <c r="J78" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K78" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M78" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L78" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16">
         <v>118</v>
       </c>
@@ -15899,14 +16267,17 @@
       <c r="I79" s="2" t="s">
         <v>743</v>
       </c>
+      <c r="J79" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M79" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <v>121</v>
       </c>
@@ -15931,14 +16302,17 @@
       <c r="I80" s="2" t="s">
         <v>762</v>
       </c>
+      <c r="J80" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K80" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M80" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <v>124</v>
       </c>
@@ -15966,14 +16340,17 @@
       <c r="I81" s="2" t="s">
         <v>782</v>
       </c>
+      <c r="J81" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K81" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M81" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L81" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
         <v>127</v>
       </c>
@@ -16001,14 +16378,17 @@
       <c r="I82" s="2" t="s">
         <v>802</v>
       </c>
+      <c r="J82" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K82" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M82" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <v>128</v>
       </c>
@@ -16036,14 +16416,17 @@
       <c r="I83" s="2" t="s">
         <v>808</v>
       </c>
+      <c r="J83" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K83" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M83" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L83" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>131</v>
       </c>
@@ -16071,14 +16454,17 @@
       <c r="I84" s="2" t="s">
         <v>828</v>
       </c>
+      <c r="J84" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K84" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M84" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L84" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16">
         <v>132</v>
       </c>
@@ -16103,14 +16489,17 @@
       <c r="I85" s="2" t="s">
         <v>833</v>
       </c>
+      <c r="J85" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K85" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M85" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16">
         <v>134</v>
       </c>
@@ -16138,14 +16527,17 @@
       <c r="I86" s="2" t="s">
         <v>844</v>
       </c>
+      <c r="J86" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K86" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M86" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L86" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16">
         <v>138</v>
       </c>
@@ -16173,14 +16565,17 @@
       <c r="I87" s="2" t="s">
         <v>871</v>
       </c>
+      <c r="J87" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K87" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M87" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16">
         <v>139</v>
       </c>
@@ -16208,14 +16603,17 @@
       <c r="I88" s="2" t="s">
         <v>877</v>
       </c>
+      <c r="J88" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K88" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M88" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L88" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>141</v>
       </c>
@@ -16243,14 +16641,17 @@
       <c r="I89" s="2" t="s">
         <v>888</v>
       </c>
+      <c r="J89" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K89" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M89" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L89" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16">
         <v>144</v>
       </c>
@@ -16278,14 +16679,17 @@
       <c r="I90" s="2" t="s">
         <v>907</v>
       </c>
+      <c r="J90" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K90" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M90" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L90" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>145</v>
       </c>
@@ -16310,14 +16714,17 @@
       <c r="I91" s="2" t="s">
         <v>912</v>
       </c>
+      <c r="J91" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K91" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M91" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L91" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16">
         <v>147</v>
       </c>
@@ -16345,14 +16752,17 @@
       <c r="I92" s="2" t="s">
         <v>923</v>
       </c>
+      <c r="J92" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K92" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M92" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L92" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16">
         <v>164</v>
       </c>
@@ -16380,14 +16790,17 @@
       <c r="I93" s="2" t="s">
         <v>1035</v>
       </c>
+      <c r="J93" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K93" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M93" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L93" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16">
         <v>174</v>
       </c>
@@ -16415,14 +16828,17 @@
       <c r="I94" s="2" t="s">
         <v>1101</v>
       </c>
+      <c r="J94" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K94" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M94" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1019" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1200</v>
+      </c>
+      <c r="L94" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1016" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="16">
         <v>185</v>
       </c>
@@ -16447,14 +16863,17 @@
       <c r="I95" s="2" t="s">
         <v>1169</v>
       </c>
+      <c r="J95" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="K95" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M95" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1019" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="L95" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1016" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="47">
         <f>COUNT(A3:A95)</f>
         <v>93</v>
@@ -16466,8 +16885,7 @@
       <c r="H96" s="56"/>
       <c r="I96" s="48"/>
       <c r="J96" s="48"/>
-      <c r="K96" s="48"/>
-      <c r="AME96"/>
+      <c r="AMB96"/>
     </row>
     <row r="97" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>

</xml_diff>

<commit_message>
Finish keywording phase 1
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD5D572-25B2-4980-B706-D23BEECA7AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B37E128-234B-45C5-9CB7-8E2CB7DBF2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="1314">
   <si>
     <t>Material search results</t>
   </si>
@@ -3960,6 +3960,42 @@
   </si>
   <si>
     <t>OpenCog, Grammar learning, Unsupervised learning, NLP, Baby Turing Test</t>
+  </si>
+  <si>
+    <t>AGI, Probabilistic programming, Genetic algorithms, Robot, Planning, Optimization, NAO</t>
+  </si>
+  <si>
+    <t>NARS, Diagnostics, Model Based Diagnostics</t>
+  </si>
+  <si>
+    <t>DSO-CA, Cognitive architectures, Global Workspace Theory, Traffic control problem</t>
+  </si>
+  <si>
+    <t>Induction, Compression, Universal search, AGI, Lifelong learning</t>
+  </si>
+  <si>
+    <t>NARS, AGI, OpenNARS, Cognitive architecture</t>
+  </si>
+  <si>
+    <t>Check if this is the first NARS paper!</t>
+  </si>
+  <si>
+    <t>Incremental compression, Universal induction, Universal search</t>
+  </si>
+  <si>
+    <t>AI aligment, AI safety, AI ethics, Ethical goal function, Control problem, AGI</t>
+  </si>
+  <si>
+    <t>Incremental compression, Hierarchical compression, Universal induction, Power laws</t>
+  </si>
+  <si>
+    <t>SP, VR, PP?</t>
+  </si>
+  <si>
+    <t>SP, VR; PP?</t>
+  </si>
+  <si>
+    <t>Reinforcement learning, Wireheading problem, Value reinforcement learning, General agent, Agent goals</t>
   </si>
 </sst>
 </file>
@@ -13641,8 +13677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M87" sqref="M87"/>
+    <sheetView tabSelected="1" topLeftCell="I67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17102,7 +17138,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <v>124</v>
       </c>
@@ -17146,7 +17182,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
         <v>127</v>
       </c>
@@ -17190,7 +17226,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <v>128</v>
       </c>
@@ -17234,7 +17270,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>131</v>
       </c>
@@ -17278,7 +17314,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16">
         <v>132</v>
       </c>
@@ -17319,7 +17355,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16">
         <v>134</v>
       </c>
@@ -17363,7 +17399,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16">
         <v>138</v>
       </c>
@@ -17400,8 +17436,14 @@
       <c r="L87" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M87" t="s">
+        <v>1302</v>
+      </c>
+      <c r="N87" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16">
         <v>139</v>
       </c>
@@ -17438,8 +17480,14 @@
       <c r="L88" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M88" t="s">
+        <v>1303</v>
+      </c>
+      <c r="N88" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>141</v>
       </c>
@@ -17476,8 +17524,14 @@
       <c r="L89" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M89" t="s">
+        <v>1304</v>
+      </c>
+      <c r="N89" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16">
         <v>144</v>
       </c>
@@ -17514,8 +17568,14 @@
       <c r="L90" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M90" t="s">
+        <v>1305</v>
+      </c>
+      <c r="N90" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>145</v>
       </c>
@@ -17549,8 +17609,17 @@
       <c r="L91" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M91" t="s">
+        <v>1306</v>
+      </c>
+      <c r="N91" t="s">
+        <v>1208</v>
+      </c>
+      <c r="P91" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16">
         <v>147</v>
       </c>
@@ -17587,8 +17656,14 @@
       <c r="L92" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M92" t="s">
+        <v>1308</v>
+      </c>
+      <c r="N92" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16">
         <v>164</v>
       </c>
@@ -17625,8 +17700,14 @@
       <c r="L93" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M93" t="s">
+        <v>1309</v>
+      </c>
+      <c r="N93" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16">
         <v>174</v>
       </c>
@@ -17663,8 +17744,14 @@
       <c r="L94" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M94" t="s">
+        <v>1310</v>
+      </c>
+      <c r="N94" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16">
         <v>185</v>
       </c>
@@ -17698,8 +17785,14 @@
       <c r="L95" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M95" t="s">
+        <v>1313</v>
+      </c>
+      <c r="N95" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="47">
         <f>COUNT(A3:A95)</f>
         <v>93</v>
@@ -17713,7 +17806,7 @@
       <c r="J96" s="48"/>
       <c r="M96" s="49">
         <f>COUNTIF(M3:M95,"&lt;&gt;")</f>
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Prepare for categorization phase 2
- Script for counting keywords, categories
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A87F8C-8E7D-4664-B798-0E00412A11FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7546E8E-8001-4B0F-B46E-A70662216925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="1647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="1654">
   <si>
     <t>Material search results</t>
   </si>
@@ -4861,6 +4861,9 @@
     <t>Different keywords</t>
   </si>
   <si>
+    <t>Total instances (Python)</t>
+  </si>
+  <si>
     <t>Cognitive architectures</t>
   </si>
   <si>
@@ -4900,6 +4903,9 @@
     <t>Homeostatic agents</t>
   </si>
   <si>
+    <t>Category theory</t>
+  </si>
+  <si>
     <t>AIXI</t>
   </si>
   <si>
@@ -4927,6 +4933,9 @@
     <t>Game playing</t>
   </si>
   <si>
+    <t>Rewarding</t>
+  </si>
+  <si>
     <t>Probabilistic approaches</t>
   </si>
   <si>
@@ -4948,34 +4957,46 @@
     <t>Agent environment</t>
   </si>
   <si>
+    <t>Question answering</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>Philosophical aspects</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>Temporal reasoning</t>
+  </si>
+  <si>
     <t>Causal reasoning</t>
   </si>
   <si>
     <t>Inference</t>
   </si>
   <si>
-    <t>NLP</t>
-  </si>
-  <si>
-    <t>Temporal reasoning</t>
-  </si>
-  <si>
     <t>Functional programming approach</t>
   </si>
   <si>
-    <t>Problemsolving?</t>
+    <t>Problemsolving</t>
   </si>
   <si>
     <t>Bio-inspired approaches</t>
   </si>
   <si>
-    <t>Reasoning</t>
+    <t>Game Theory</t>
   </si>
   <si>
     <t>Physical robots</t>
   </si>
   <si>
-    <t>Total instances (Python)</t>
+    <t>Diagnostics</t>
+  </si>
+  <si>
+    <t>Categorization phase 2</t>
   </si>
 </sst>
 </file>
@@ -4988,7 +5009,7 @@
     <numFmt numFmtId="166" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5067,8 +5088,16 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5146,8 +5175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -5233,8 +5268,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -5265,8 +5309,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5348,10 +5393,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="30"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="31">
     <cellStyle name="Accent 1 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Bad 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -5381,6 +5430,7 @@
     <cellStyle name="Neutral 8" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Neutral 9" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Otsikko 2" xfId="30" builtinId="17"/>
     <cellStyle name="Otsikko 4" xfId="2" builtinId="19"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -14688,8 +14738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="J68" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M88" sqref="M88"/>
+    <sheetView topLeftCell="F19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20386,10 +20436,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q299"/>
+  <dimension ref="A1:S299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F277" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O298" sqref="O298"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20399,7 +20449,7 @@
     <col min="3" max="3" width="42.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -20408,9 +20458,12 @@
     <col min="12" max="12" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" style="46"/>
+    <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>1605</v>
       </c>
@@ -20418,15 +20471,15 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P2" t="s">
         <v>1607</v>
       </c>
       <c r="Q2" t="s">
-        <v>1646</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="36" t="s">
         <v>1310</v>
@@ -20444,13 +20497,14 @@
         <f t="shared" ref="P3:P15" si="0">COUNTIF(B3:O3,"&lt;&gt;")</f>
         <v>4</v>
       </c>
-      <c r="Q3" s="44">
+      <c r="Q3" s="43">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3" s="47"/>
+    </row>
+    <row r="4" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="B4" t="s">
         <v>1311</v>
@@ -20470,17 +20524,23 @@
       <c r="G4" t="s">
         <v>1405</v>
       </c>
+      <c r="H4" t="s">
+        <v>1331</v>
+      </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>20</v>
+      </c>
+      <c r="S4" s="45" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="B5" t="s">
         <v>1312</v>
@@ -20492,13 +20552,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="Q5" s="44">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="B6" t="s">
         <v>1314</v>
@@ -20519,25 +20579,22 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="Q6" s="44">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>1331</v>
-      </c>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="B8" t="s">
         <v>1313</v>
@@ -20564,11 +20621,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q8" s="43">
+      <c r="Q8" s="44">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -20577,9 +20634,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="B10" t="s">
         <v>1317</v>
@@ -20603,13 +20660,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="44">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B11" t="s">
         <v>1318</v>
@@ -20648,13 +20705,13 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="Q11" s="43">
+      <c r="Q11" s="44">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B12" t="s">
         <v>1319</v>
@@ -20672,13 +20729,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Q12" s="43">
+      <c r="Q12" s="44">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B13" t="s">
         <v>1323</v>
@@ -20705,13 +20762,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="Q13" s="44">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="B14" t="s">
         <v>1321</v>
@@ -20732,13 +20789,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="44">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B15" t="s">
         <v>1322</v>
@@ -20752,22 +20809,25 @@
       <c r="E15" t="s">
         <v>1494</v>
       </c>
+      <c r="F15" t="s">
+        <v>1474</v>
+      </c>
       <c r="P15">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q15" s="43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="Q16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="B17" t="s">
         <v>1324</v>
@@ -20791,13 +20851,13 @@
         <f t="shared" ref="P17:P48" si="1">COUNTIF(B17:O17,"&lt;&gt;")</f>
         <v>6</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="Q17" s="44">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="B18" t="s">
         <v>1325</v>
@@ -20821,7 +20881,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="Q18" s="44">
         <v>11</v>
       </c>
     </row>
@@ -20836,7 +20896,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="B20" t="s">
         <v>1327</v>
@@ -20863,7 +20923,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="Q20" s="43">
+      <c r="Q20" s="44">
         <v>12</v>
       </c>
     </row>
@@ -20877,6 +20937,9 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
+        <v>1622</v>
+      </c>
       <c r="B22" t="s">
         <v>1328</v>
       </c>
@@ -20908,7 +20971,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="B25" t="s">
         <v>1316</v>
@@ -20920,13 +20983,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q25" s="43">
+      <c r="Q25" s="44">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="B26" t="s">
         <v>1333</v>
@@ -20953,13 +21016,13 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="Q26" s="43">
+      <c r="Q26" s="44">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="B27" t="s">
         <v>1334</v>
@@ -20974,7 +21037,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Q27" s="43">
+      <c r="Q27" s="44">
         <v>5</v>
       </c>
     </row>
@@ -20992,7 +21055,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Q28" s="43">
+      <c r="Q28" s="44">
         <v>6</v>
       </c>
     </row>
@@ -21007,7 +21070,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>1624</v>
+        <v>1626</v>
       </c>
       <c r="B30" t="s">
         <v>1337</v>
@@ -21021,17 +21084,20 @@
       <c r="E30" t="s">
         <v>1417</v>
       </c>
+      <c r="F30" t="s">
+        <v>1426</v>
+      </c>
       <c r="P30">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q30" s="43">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="Q30" s="44">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="B31" t="s">
         <v>1338</v>
@@ -21049,7 +21115,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q31" s="43">
+      <c r="Q31" s="44">
         <v>6</v>
       </c>
     </row>
@@ -21082,7 +21148,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="B35" t="s">
         <v>1342</v>
@@ -21099,17 +21165,26 @@
       <c r="F35" t="s">
         <v>1466</v>
       </c>
+      <c r="G35" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1380</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1503</v>
+      </c>
       <c r="P35">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="Q35" s="43">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="Q35" s="44">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>1627</v>
+        <v>1629</v>
       </c>
       <c r="B36" t="s">
         <v>1343</v>
@@ -21145,7 +21220,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
-        <v>1628</v>
+        <v>1630</v>
       </c>
       <c r="B39" t="s">
         <v>1344</v>
@@ -21160,13 +21235,13 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="B40" t="s">
         <v>1340</v>
@@ -21190,7 +21265,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="Q40" s="43">
+      <c r="Q40" s="44">
         <v>7</v>
       </c>
     </row>
@@ -21204,15 +21279,12 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>1384</v>
-      </c>
       <c r="P42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -21234,6 +21306,9 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="38" t="s">
+        <v>1632</v>
+      </c>
       <c r="B45" t="s">
         <v>1352</v>
       </c>
@@ -21271,7 +21346,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="B48" t="s">
         <v>1355</v>
@@ -21289,7 +21364,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q48" s="43">
+      <c r="Q48" s="44">
         <v>5</v>
       </c>
     </row>
@@ -21304,7 +21379,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
       <c r="B50" t="s">
         <v>1418</v>
@@ -21364,7 +21439,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
-        <v>1632</v>
+        <v>1635</v>
       </c>
       <c r="B55" t="s">
         <v>1362</v>
@@ -21379,7 +21454,7 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="44">
         <v>4</v>
       </c>
     </row>
@@ -21394,7 +21469,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="s">
-        <v>1633</v>
+        <v>1636</v>
       </c>
       <c r="B57" t="s">
         <v>1364</v>
@@ -21421,13 +21496,13 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Q57" s="43">
+      <c r="Q57" s="44">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
-        <v>1634</v>
+        <v>1637</v>
       </c>
       <c r="B58" t="s">
         <v>1543</v>
@@ -21463,7 +21538,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="38" t="s">
-        <v>1635</v>
+        <v>1638</v>
       </c>
       <c r="B61" t="s">
         <v>1368</v>
@@ -21487,7 +21562,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Q61" s="43">
+      <c r="Q61" s="44">
         <v>7</v>
       </c>
     </row>
@@ -21510,15 +21585,12 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>1371</v>
-      </c>
       <c r="P64">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -21532,7 +21604,7 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="38" t="s">
-        <v>1636</v>
+        <v>1639</v>
       </c>
       <c r="B66" t="s">
         <v>1385</v>
@@ -21555,33 +21627,39 @@
       <c r="H66" t="s">
         <v>1516</v>
       </c>
+      <c r="I66" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J66" t="s">
+        <v>1384</v>
+      </c>
       <c r="P66">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="Q66" s="43">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="Q66" s="44">
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>1402</v>
-      </c>
       <c r="P67">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>1371</v>
+      </c>
       <c r="P68">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -21606,18 +21684,12 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
-        <v>1378</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1380</v>
-      </c>
       <c r="P71">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q71">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -21672,52 +21744,18 @@
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77" s="38" t="s">
-        <v>1637</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1507</v>
-      </c>
-      <c r="C77" t="s">
-        <v>1544</v>
-      </c>
-      <c r="D77" t="s">
-        <v>1489</v>
-      </c>
       <c r="Q77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="38" t="s">
-        <v>1638</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1438</v>
-      </c>
-      <c r="C78" t="s">
-        <v>1579</v>
-      </c>
-      <c r="D78" t="s">
-        <v>1367</v>
-      </c>
-      <c r="E78" t="s">
-        <v>1505</v>
-      </c>
-      <c r="F78" t="s">
-        <v>1518</v>
-      </c>
-      <c r="P78">
-        <f t="shared" ref="P78:P110" si="3">COUNTIF(B78:O78,"&lt;&gt;")</f>
-        <v>5</v>
-      </c>
-      <c r="Q78" s="43">
-        <v>6</v>
+      <c r="Q78">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P79">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="P79:P110" si="3">COUNTIF(B79:O79,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q79">
@@ -21725,6 +21763,9 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="38" t="s">
+        <v>1640</v>
+      </c>
       <c r="B80" t="s">
         <v>1387</v>
       </c>
@@ -21744,7 +21785,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="Q80" s="43">
+      <c r="Q80" s="44">
         <v>5</v>
       </c>
     </row>
@@ -21759,7 +21800,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="38" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
       <c r="B82" t="s">
         <v>1389</v>
@@ -21821,30 +21862,36 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="38" t="s">
+        <v>1642</v>
+      </c>
       <c r="B87" t="s">
         <v>1394</v>
       </c>
       <c r="C87" t="s">
         <v>1433</v>
       </c>
+      <c r="D87" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1357</v>
+      </c>
       <c r="P87">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="Q87">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="Q87" s="44">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>1357</v>
-      </c>
       <c r="P88">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q88">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -22013,39 +22060,39 @@
       <c r="B106" t="s">
         <v>1413</v>
       </c>
-      <c r="C106" t="s">
-        <v>1412</v>
-      </c>
-      <c r="D106" t="s">
-        <v>1407</v>
-      </c>
-      <c r="E106" t="s">
-        <v>1415</v>
-      </c>
       <c r="P106">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q106">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1407</v>
+      </c>
       <c r="P107">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q107">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>1415</v>
+      </c>
       <c r="P108">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:17" x14ac:dyDescent="0.2">
@@ -22153,18 +22200,12 @@
       </c>
     </row>
     <row r="119" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B119" t="s">
-        <v>1426</v>
-      </c>
-      <c r="C119" t="s">
-        <v>1428</v>
-      </c>
       <c r="P119">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q119">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:17" x14ac:dyDescent="0.2">
@@ -22180,12 +22221,15 @@
       </c>
     </row>
     <row r="121" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>1428</v>
+      </c>
       <c r="P121">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:17" x14ac:dyDescent="0.2">
@@ -22306,15 +22350,12 @@
       <c r="B134" t="s">
         <v>1441</v>
       </c>
-      <c r="C134" t="s">
-        <v>1444</v>
-      </c>
       <c r="P134">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q134">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="2:17" x14ac:dyDescent="0.2">
@@ -22585,15 +22626,12 @@
       </c>
     </row>
     <row r="162" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B162" t="s">
-        <v>1469</v>
-      </c>
       <c r="P162">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="2:17" x14ac:dyDescent="0.2">
@@ -22642,15 +22680,12 @@
       </c>
     </row>
     <row r="167" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B167" t="s">
-        <v>1474</v>
-      </c>
       <c r="P167">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="2:17" x14ac:dyDescent="0.2">
@@ -22759,41 +22794,48 @@
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P178">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="Q178">
         <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B179" t="s">
-        <v>1486</v>
-      </c>
-      <c r="P179">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
       <c r="Q179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A180" s="38" t="s">
+        <v>1643</v>
+      </c>
       <c r="B180" t="s">
-        <v>1487</v>
+        <v>1564</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G180" t="s">
+        <v>1498</v>
       </c>
       <c r="P180">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Q180">
-        <v>1</v>
+        <f>COUNTIF(B180:O180,"&lt;&gt;")</f>
+        <v>6</v>
+      </c>
+      <c r="Q180" s="44">
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" s="38" t="s">
-        <v>1640</v>
+        <v>1644</v>
       </c>
       <c r="B181" t="s">
         <v>1488</v>
@@ -22805,7 +22847,7 @@
         <v>1553</v>
       </c>
       <c r="P181">
-        <f t="shared" si="6"/>
+        <f>COUNTIF(B181:O181,"&lt;&gt;")</f>
         <v>3</v>
       </c>
       <c r="Q181">
@@ -22813,28 +22855,50 @@
       </c>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P182">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="A182" s="38" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1489</v>
       </c>
       <c r="Q182">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A183" s="38" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E183" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1518</v>
+      </c>
       <c r="P183">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q183">
-        <v>0</v>
+        <f>COUNTIF(B183:O183,"&lt;&gt;")</f>
+        <v>5</v>
+      </c>
+      <c r="Q183" s="44">
+        <v>6</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P184">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="Q184">
         <v>0</v>
       </c>
@@ -22844,7 +22908,7 @@
         <v>1492</v>
       </c>
       <c r="P185">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="P185:P216" si="7">COUNTIF(B185:O185,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="Q185">
@@ -22855,29 +22919,29 @@
       <c r="B186" t="s">
         <v>1493</v>
       </c>
-      <c r="C186" t="s">
+      <c r="P186">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B187" t="s">
         <v>1495</v>
       </c>
-      <c r="P186">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="Q186">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P187">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="Q187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P188">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q188">
@@ -22892,7 +22956,7 @@
         <v>1497</v>
       </c>
       <c r="P189">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="Q189">
@@ -22901,7 +22965,7 @@
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P190">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q190">
@@ -22910,7 +22974,7 @@
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P191">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q191">
@@ -22919,7 +22983,7 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P192">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q192">
@@ -22933,20 +22997,17 @@
       <c r="C193" t="s">
         <v>1501</v>
       </c>
-      <c r="D193" t="s">
-        <v>1503</v>
-      </c>
       <c r="P193">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="Q193">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P194">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q194">
@@ -22958,7 +23019,7 @@
         <v>1502</v>
       </c>
       <c r="P195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q195">
@@ -22967,7 +23028,7 @@
     </row>
     <row r="196" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P196">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q196">
@@ -22979,7 +23040,7 @@
         <v>1504</v>
       </c>
       <c r="P197">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q197">
@@ -22988,7 +23049,7 @@
     </row>
     <row r="198" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P198">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q198">
@@ -23000,7 +23061,7 @@
         <v>1506</v>
       </c>
       <c r="P199">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q199">
@@ -23009,7 +23070,7 @@
     </row>
     <row r="200" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P200">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q200">
@@ -23018,7 +23079,7 @@
     </row>
     <row r="201" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P201">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q201">
@@ -23030,7 +23091,7 @@
         <v>1509</v>
       </c>
       <c r="P202">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q202">
@@ -23042,7 +23103,7 @@
         <v>1510</v>
       </c>
       <c r="P203">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q203">
@@ -23051,7 +23112,7 @@
     </row>
     <row r="204" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q204">
@@ -23066,7 +23127,7 @@
         <v>1511</v>
       </c>
       <c r="P205">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="Q205">
@@ -23075,7 +23136,7 @@
     </row>
     <row r="206" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P206">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q206">
@@ -23083,21 +23144,27 @@
       </c>
     </row>
     <row r="207" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
+        <v>1487</v>
+      </c>
       <c r="P207">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="Q207">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
+        <v>1486</v>
+      </c>
       <c r="P208">
-        <f t="shared" ref="P208:P239" si="7">COUNTIF(B208:O208,"&lt;&gt;")</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="Q208">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.2">
@@ -23174,7 +23241,7 @@
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P217">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="P217:P248" si="8">COUNTIF(B217:O217,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q217">
@@ -23186,7 +23253,7 @@
         <v>1525</v>
       </c>
       <c r="P218">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q218">
@@ -23195,7 +23262,7 @@
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="38" t="s">
-        <v>1641</v>
+        <v>1647</v>
       </c>
       <c r="B219" t="s">
         <v>1526</v>
@@ -23207,7 +23274,7 @@
         <v>1555</v>
       </c>
       <c r="P219">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="Q219">
@@ -23216,7 +23283,7 @@
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P220">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q220">
@@ -23225,7 +23292,7 @@
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P221">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q221">
@@ -23237,7 +23304,7 @@
         <v>1529</v>
       </c>
       <c r="P222">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q222">
@@ -23249,7 +23316,7 @@
         <v>1530</v>
       </c>
       <c r="P223">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q223">
@@ -23261,7 +23328,7 @@
         <v>1531</v>
       </c>
       <c r="P224">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q224">
@@ -23273,7 +23340,7 @@
         <v>1532</v>
       </c>
       <c r="P225">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q225">
@@ -23282,7 +23349,7 @@
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P226">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q226">
@@ -23294,7 +23361,7 @@
         <v>1534</v>
       </c>
       <c r="P227">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q227">
@@ -23303,7 +23370,7 @@
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P228">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q228">
@@ -23312,7 +23379,7 @@
     </row>
     <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P229">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q229">
@@ -23321,7 +23388,7 @@
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P230">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q230">
@@ -23333,7 +23400,7 @@
         <v>1538</v>
       </c>
       <c r="P231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q231">
@@ -23342,7 +23409,7 @@
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" s="38" t="s">
-        <v>1642</v>
+        <v>1648</v>
       </c>
       <c r="B232" t="s">
         <v>1539</v>
@@ -23357,10 +23424,10 @@
         <v>1499</v>
       </c>
       <c r="P232">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="Q232">
+      <c r="Q232" s="44">
         <v>4</v>
       </c>
     </row>
@@ -23369,7 +23436,7 @@
         <v>1540</v>
       </c>
       <c r="P233">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q233">
@@ -23381,7 +23448,7 @@
         <v>1541</v>
       </c>
       <c r="P234">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q234">
@@ -23393,7 +23460,7 @@
         <v>1542</v>
       </c>
       <c r="P235">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q235">
@@ -23402,7 +23469,7 @@
     </row>
     <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P236">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q236">
@@ -23411,7 +23478,7 @@
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P237">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q237">
@@ -23420,7 +23487,7 @@
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P238">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q238">
@@ -23429,7 +23496,7 @@
     </row>
     <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P239">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q239">
@@ -23438,7 +23505,7 @@
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P240">
-        <f t="shared" ref="P240:P271" si="8">COUNTIF(B240:O240,"&lt;&gt;")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q240">
@@ -23456,7 +23523,7 @@
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="38" t="s">
-        <v>1643</v>
+        <v>1649</v>
       </c>
       <c r="B242" t="s">
         <v>1549</v>
@@ -23467,12 +23534,15 @@
       <c r="D242" t="s">
         <v>1586</v>
       </c>
+      <c r="E242" t="s">
+        <v>1444</v>
+      </c>
       <c r="P242">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="Q242">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="Q242" s="44">
+        <v>4</v>
       </c>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.2">
@@ -23534,7 +23604,7 @@
     </row>
     <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P249">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="P249:P280" si="9">COUNTIF(B249:O249,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q249">
@@ -23543,7 +23613,7 @@
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P250">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q250">
@@ -23552,7 +23622,7 @@
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P251">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q251">
@@ -23561,7 +23631,7 @@
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P252">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q252">
@@ -23573,7 +23643,7 @@
         <v>1560</v>
       </c>
       <c r="P253">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q253">
@@ -23585,7 +23655,7 @@
         <v>1561</v>
       </c>
       <c r="P254">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q254">
@@ -23597,7 +23667,7 @@
         <v>1562</v>
       </c>
       <c r="P255">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q255">
@@ -23609,7 +23679,7 @@
         <v>1563</v>
       </c>
       <c r="P256">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q256">
@@ -23617,33 +23687,8 @@
       </c>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A257" s="38" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B257" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C257" t="s">
-        <v>1546</v>
-      </c>
-      <c r="D257" t="s">
-        <v>1521</v>
-      </c>
-      <c r="E257" t="s">
-        <v>1437</v>
-      </c>
-      <c r="F257" t="s">
-        <v>1547</v>
-      </c>
-      <c r="G257" t="s">
-        <v>1498</v>
-      </c>
-      <c r="P257">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="Q257" s="43">
-        <v>6</v>
+      <c r="Q257">
+        <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.2">
@@ -23654,7 +23699,7 @@
         <v>1406</v>
       </c>
       <c r="P258">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="P258:P297" si="10">COUNTIF(B258:O258,"&lt;&gt;")</f>
         <v>2</v>
       </c>
       <c r="Q258">
@@ -23663,7 +23708,7 @@
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P259">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q259">
@@ -23672,7 +23717,7 @@
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P260">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q260">
@@ -23680,6 +23725,9 @@
       </c>
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A261" s="38" t="s">
+        <v>1650</v>
+      </c>
       <c r="B261" t="s">
         <v>1568</v>
       </c>
@@ -23687,7 +23735,7 @@
         <v>1569</v>
       </c>
       <c r="P261">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="Q261">
@@ -23696,7 +23744,7 @@
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P262">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q262">
@@ -23708,7 +23756,7 @@
         <v>1570</v>
       </c>
       <c r="P263">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q263">
@@ -23720,7 +23768,7 @@
         <v>1571</v>
       </c>
       <c r="P264">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q264">
@@ -23729,7 +23777,7 @@
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P265">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q265">
@@ -23738,7 +23786,7 @@
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P266">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q266">
@@ -23750,7 +23798,7 @@
         <v>1574</v>
       </c>
       <c r="P267">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q267">
@@ -23762,7 +23810,7 @@
         <v>1575</v>
       </c>
       <c r="P268">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q268">
@@ -23777,7 +23825,7 @@
         <v>1578</v>
       </c>
       <c r="P269">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="Q269">
@@ -23786,7 +23834,7 @@
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P270">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q270">
@@ -23795,7 +23843,7 @@
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P271">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q271">
@@ -23804,7 +23852,7 @@
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P272">
-        <f t="shared" ref="P272:P303" si="9">COUNTIF(B272:O272,"&lt;&gt;")</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q272">
@@ -23813,7 +23861,7 @@
     </row>
     <row r="273" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P273">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q273">
@@ -23825,7 +23873,7 @@
         <v>1580</v>
       </c>
       <c r="P274">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q274">
@@ -23837,7 +23885,7 @@
         <v>1581</v>
       </c>
       <c r="P275">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q275">
@@ -23846,7 +23894,7 @@
     </row>
     <row r="276" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P276">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q276">
@@ -23855,7 +23903,7 @@
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P277">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q277">
@@ -23864,7 +23912,7 @@
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P278">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q278">
@@ -23873,7 +23921,7 @@
     </row>
     <row r="279" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P279">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q279">
@@ -23882,7 +23930,7 @@
     </row>
     <row r="280" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P280">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q280">
@@ -23891,7 +23939,7 @@
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A281" s="38" t="s">
-        <v>1645</v>
+        <v>1651</v>
       </c>
       <c r="B281" t="s">
         <v>1587</v>
@@ -23906,16 +23954,16 @@
         <v>1445</v>
       </c>
       <c r="P281">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="Q281">
+      <c r="Q281" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P282">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q282">
@@ -23923,6 +23971,9 @@
       </c>
     </row>
     <row r="283" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A283" s="38" t="s">
+        <v>1652</v>
+      </c>
       <c r="B283" t="s">
         <v>1589</v>
       </c>
@@ -23930,7 +23981,7 @@
         <v>1590</v>
       </c>
       <c r="P283">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="Q283">
@@ -23939,7 +23990,7 @@
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P284">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q284">
@@ -23948,7 +23999,7 @@
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P285">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q285">
@@ -23957,7 +24008,7 @@
     </row>
     <row r="286" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P286">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q286">
@@ -23969,7 +24020,7 @@
         <v>1593</v>
       </c>
       <c r="P287">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q287">
@@ -23978,123 +24029,124 @@
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P288">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q288">
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P289">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q289">
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P290">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q290">
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P291">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q291">
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P292">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q292">
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P293">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q293">
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B294" t="s">
         <v>1600</v>
       </c>
       <c r="P294">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q294">
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P295">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q295">
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P296">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q296">
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P297">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q297">
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298" s="40">
         <f>COUNTIF(A3:A297, "&lt;&gt;")</f>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B298" s="34">
         <f>COUNTIF(B3:B297,"&lt;&gt;")</f>
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P298" s="34">
         <f>COUNTIF(P3:P297,"&gt;1")</f>
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Q298" s="34">
         <f>COUNTIF(Q3:Q297,"&gt;1")</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="R298" s="48"/>
+    </row>
+    <row r="299" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P299" s="34">
         <f>COUNTIF(P4:P298,"&gt;4")</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q299" s="34">
-        <f>COUNTIF(Q4:Q298,"&gt;4")</f>
-        <v>29</v>
+        <f>COUNTIF(Q4:Q298,"&gt;=4")</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start merging of categories
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7546E8E-8001-4B0F-B46E-A70662216925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65726B5B-D9AC-414F-83CE-288121EF290A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="1654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="1654">
   <si>
     <t>Material search results</t>
   </si>
@@ -4867,6 +4867,9 @@
     <t>Cognitive architectures</t>
   </si>
   <si>
+    <t>Categorization phase 2</t>
+  </si>
+  <si>
     <t>NARS</t>
   </si>
   <si>
@@ -4891,6 +4894,9 @@
     <t>RSI</t>
   </si>
   <si>
+    <t>Universal Induction</t>
+  </si>
+  <si>
     <t>Multi-agent systems</t>
   </si>
   <si>
@@ -4909,7 +4915,7 @@
     <t>AIXI</t>
   </si>
   <si>
-    <t>Universal Induction</t>
+    <t>Planning &amp; decision making</t>
   </si>
   <si>
     <t>Compression</t>
@@ -4921,6 +4927,9 @@
     <t>AGI design</t>
   </si>
   <si>
+    <t>Agent environment</t>
+  </si>
+  <si>
     <t>AI research</t>
   </si>
   <si>
@@ -4933,70 +4942,61 @@
     <t>Game playing</t>
   </si>
   <si>
+    <t>Philosophical aspects</t>
+  </si>
+  <si>
     <t>Rewarding</t>
   </si>
   <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
     <t>Probabilistic approaches</t>
   </si>
   <si>
+    <t>Inference</t>
+  </si>
+  <si>
     <t>Neural networks</t>
   </si>
   <si>
+    <t>Artificial pedagogy</t>
+  </si>
+  <si>
     <t>Understanding</t>
   </si>
   <si>
-    <t>Artificial pedagogy</t>
-  </si>
-  <si>
     <t>Imitation learning</t>
   </si>
   <si>
-    <t>Planning &amp; decision making</t>
-  </si>
-  <si>
-    <t>Agent environment</t>
+    <t>Problemsolving</t>
+  </si>
+  <si>
+    <t>Bio-inspired approaches</t>
+  </si>
+  <si>
+    <t>Physical robots</t>
+  </si>
+  <si>
+    <t>Causal reasoning</t>
+  </si>
+  <si>
+    <t>NLP</t>
   </si>
   <si>
     <t>Question answering</t>
   </si>
   <si>
-    <t>NLP</t>
-  </si>
-  <si>
-    <t>Philosophical aspects</t>
-  </si>
-  <si>
-    <t>Reasoning</t>
-  </si>
-  <si>
     <t>Temporal reasoning</t>
   </si>
   <si>
-    <t>Causal reasoning</t>
-  </si>
-  <si>
-    <t>Inference</t>
-  </si>
-  <si>
     <t>Functional programming approach</t>
   </si>
   <si>
-    <t>Problemsolving</t>
-  </si>
-  <si>
-    <t>Bio-inspired approaches</t>
-  </si>
-  <si>
     <t>Game Theory</t>
   </si>
   <si>
-    <t>Physical robots</t>
-  </si>
-  <si>
     <t>Diagnostics</t>
-  </si>
-  <si>
-    <t>Categorization phase 2</t>
   </si>
 </sst>
 </file>
@@ -5309,7 +5309,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -20436,10 +20436,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S299"/>
+  <dimension ref="A1:AD299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="L43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y59" sqref="Y59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20458,12 +20458,13 @@
     <col min="12" max="12" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="46"/>
-    <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" style="46" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>1605</v>
       </c>
@@ -20471,7 +20472,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P2" t="s">
         <v>1607</v>
       </c>
@@ -20479,7 +20480,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="36" t="s">
         <v>1310</v>
@@ -20502,7 +20503,7 @@
       </c>
       <c r="R3" s="47"/>
     </row>
-    <row r="4" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
         <v>1609</v>
       </c>
@@ -20535,12 +20536,12 @@
         <v>20</v>
       </c>
       <c r="S4" s="45" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="B5" t="s">
         <v>1312</v>
@@ -20556,9 +20557,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="B6" t="s">
         <v>1314</v>
@@ -20582,8 +20583,14 @@
       <c r="Q6" s="44">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>1609</v>
+      </c>
+      <c r="U6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -20591,10 +20598,16 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="U7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="B8" t="s">
         <v>1313</v>
@@ -20624,8 +20637,14 @@
       <c r="Q8" s="44">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>1612</v>
+      </c>
+      <c r="U8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -20634,9 +20653,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B10" t="s">
         <v>1317</v>
@@ -20663,10 +20682,16 @@
       <c r="Q10" s="44">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>1615</v>
+      </c>
+      <c r="U10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B11" t="s">
         <v>1318</v>
@@ -20708,10 +20733,16 @@
       <c r="Q11" s="44">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>1618</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B12" t="s">
         <v>1319</v>
@@ -20732,10 +20763,16 @@
       <c r="Q12" s="44">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="X12" t="s">
+        <v>1613</v>
+      </c>
+      <c r="Y12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="B13" t="s">
         <v>1323</v>
@@ -20766,9 +20803,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B14" t="s">
         <v>1321</v>
@@ -20792,10 +20829,16 @@
       <c r="Q14" s="44">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>1619</v>
+      </c>
+      <c r="U14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
-        <v>1618</v>
+        <v>1620</v>
       </c>
       <c r="B15" t="s">
         <v>1322</v>
@@ -20819,15 +20862,27 @@
       <c r="Q15" s="44">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>1625</v>
+      </c>
+      <c r="U15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T16" t="s">
+        <v>1627</v>
+      </c>
+      <c r="U16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="B17" t="s">
         <v>1324</v>
@@ -20855,9 +20910,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="B18" t="s">
         <v>1325</v>
@@ -20884,8 +20939,14 @@
       <c r="Q18" s="44">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>1621</v>
+      </c>
+      <c r="U18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P19">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -20894,9 +20955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="B20" t="s">
         <v>1327</v>
@@ -20926,8 +20987,14 @@
       <c r="Q20" s="44">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T20" t="s">
+        <v>1626</v>
+      </c>
+      <c r="U20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -20936,9 +21003,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="B22" t="s">
         <v>1328</v>
@@ -20950,8 +21017,14 @@
       <c r="Q22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>1617</v>
+      </c>
+      <c r="U22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P23">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -20960,7 +21033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P24">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -20968,10 +21041,16 @@
       <c r="Q24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>1614</v>
+      </c>
+      <c r="U24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="B25" t="s">
         <v>1316</v>
@@ -20986,10 +21065,16 @@
       <c r="Q25" s="44">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T25" t="s">
+        <v>1630</v>
+      </c>
+      <c r="U25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
-        <v>1624</v>
+        <v>1619</v>
       </c>
       <c r="B26" t="s">
         <v>1333</v>
@@ -21019,10 +21104,16 @@
       <c r="Q26" s="44">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T26" t="s">
+        <v>1633</v>
+      </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="B27" t="s">
         <v>1334</v>
@@ -21041,7 +21132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>1349</v>
       </c>
@@ -21058,8 +21149,14 @@
       <c r="Q28" s="44">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T28" t="s">
+        <v>1628</v>
+      </c>
+      <c r="U28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P29">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21068,9 +21165,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="B30" t="s">
         <v>1337</v>
@@ -21094,10 +21191,16 @@
       <c r="Q30" s="44">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T30" t="s">
+        <v>1629</v>
+      </c>
+      <c r="U30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>1627</v>
+        <v>1629</v>
       </c>
       <c r="B31" t="s">
         <v>1338</v>
@@ -21119,7 +21222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P32">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21127,8 +21230,14 @@
       <c r="Q32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T32" t="s">
+        <v>1622</v>
+      </c>
+      <c r="U32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P33">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21137,7 +21246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P34">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21145,10 +21254,16 @@
       <c r="Q34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T34" t="s">
+        <v>1631</v>
+      </c>
+      <c r="U34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
-        <v>1628</v>
+        <v>1631</v>
       </c>
       <c r="B35" t="s">
         <v>1342</v>
@@ -21182,9 +21297,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="B36" t="s">
         <v>1343</v>
@@ -21200,7 +21315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P37">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21209,7 +21324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P38">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21217,10 +21332,16 @@
       <c r="Q38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T38" t="s">
+        <v>1616</v>
+      </c>
+      <c r="U38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="B39" t="s">
         <v>1344</v>
@@ -21239,9 +21360,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
       <c r="B40" t="s">
         <v>1340</v>
@@ -21269,7 +21390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P41">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21278,7 +21399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P42">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21286,8 +21407,14 @@
       <c r="Q42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T42" t="s">
+        <v>1635</v>
+      </c>
+      <c r="U42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P43">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21296,7 +21423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21304,10 +21431,16 @@
       <c r="Q44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T44" t="s">
+        <v>1620</v>
+      </c>
+      <c r="U44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
-        <v>1632</v>
+        <v>1636</v>
       </c>
       <c r="B45" t="s">
         <v>1352</v>
@@ -21323,7 +21456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P46">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21331,8 +21464,14 @@
       <c r="Q46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T46" t="s">
+        <v>1637</v>
+      </c>
+      <c r="U46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>1354</v>
       </c>
@@ -21343,10 +21482,16 @@
       <c r="Q47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T47" t="s">
+        <v>1639</v>
+      </c>
+      <c r="U47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
-        <v>1633</v>
+        <v>1638</v>
       </c>
       <c r="B48" t="s">
         <v>1355</v>
@@ -21367,8 +21512,14 @@
       <c r="Q48" s="44">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T48" t="s">
+        <v>1647</v>
+      </c>
+      <c r="U48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P49">
         <f t="shared" ref="P49:P80" si="2">COUNTIF(B49:O49,"&lt;&gt;")</f>
         <v>0</v>
@@ -21376,10 +21527,16 @@
       <c r="Q49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T49" t="s">
+        <v>1650</v>
+      </c>
+      <c r="U49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
-        <v>1634</v>
+        <v>1640</v>
       </c>
       <c r="B50" t="s">
         <v>1418</v>
@@ -21398,7 +21555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P51">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21407,7 +21564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P52">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21415,8 +21572,14 @@
       <c r="Q52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="X52" t="s">
+        <v>1638</v>
+      </c>
+      <c r="Y52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>1360</v>
       </c>
@@ -21428,7 +21591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P54">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21436,10 +21599,22 @@
       <c r="Q54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T54" t="s">
+        <v>1641</v>
+      </c>
+      <c r="U54">
+        <v>4</v>
+      </c>
+      <c r="X54" t="s">
+        <v>1623</v>
+      </c>
+      <c r="Y54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
-        <v>1635</v>
+        <v>1642</v>
       </c>
       <c r="B55" t="s">
         <v>1362</v>
@@ -21457,8 +21632,14 @@
       <c r="Q55" s="44">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="X55" t="s">
+        <v>1645</v>
+      </c>
+      <c r="Y55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P56">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21467,9 +21648,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="s">
-        <v>1636</v>
+        <v>1641</v>
       </c>
       <c r="B57" t="s">
         <v>1364</v>
@@ -21500,9 +21681,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
-        <v>1637</v>
+        <v>1643</v>
       </c>
       <c r="B58" t="s">
         <v>1543</v>
@@ -21517,8 +21698,14 @@
       <c r="Q58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T58" t="s">
+        <v>1644</v>
+      </c>
+      <c r="U58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P59">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21526,8 +21713,14 @@
       <c r="Q59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T59" t="s">
+        <v>1649</v>
+      </c>
+      <c r="U59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P60">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21535,10 +21728,16 @@
       <c r="Q60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="X60" t="s">
+        <v>1634</v>
+      </c>
+      <c r="Y60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="38" t="s">
-        <v>1638</v>
+        <v>1626</v>
       </c>
       <c r="B61" t="s">
         <v>1368</v>
@@ -21566,7 +21765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P62">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21574,8 +21773,14 @@
       <c r="Q62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T62" t="s">
+        <v>1636</v>
+      </c>
+      <c r="U62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P63">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21584,7 +21789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="P64">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21592,8 +21797,14 @@
       <c r="Q64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T64" t="s">
+        <v>1640</v>
+      </c>
+      <c r="U64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P65">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21602,9 +21813,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="38" t="s">
-        <v>1639</v>
+        <v>1630</v>
       </c>
       <c r="B66" t="s">
         <v>1385</v>
@@ -21641,7 +21852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P67">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21650,7 +21861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>1371</v>
       </c>
@@ -21661,8 +21872,14 @@
       <c r="Q68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T68" t="s">
+        <v>1646</v>
+      </c>
+      <c r="U68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P69">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21671,7 +21888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>1377</v>
       </c>
@@ -21682,8 +21899,14 @@
       <c r="Q70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T70" t="s">
+        <v>1624</v>
+      </c>
+      <c r="U70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P71">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21692,7 +21915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P72">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21701,7 +21924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>1583</v>
       </c>
@@ -21713,7 +21936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P74">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21721,8 +21944,14 @@
       <c r="Q74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T74" t="s">
+        <v>1632</v>
+      </c>
+      <c r="U74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>1366</v>
       </c>
@@ -21734,7 +21963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P76">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -21743,17 +21972,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="Q77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="Q78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T78" t="s">
+        <v>1648</v>
+      </c>
+      <c r="U78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P79">
         <f t="shared" ref="P79:P110" si="3">COUNTIF(B79:O79,"&lt;&gt;")</f>
         <v>0</v>
@@ -21762,9 +21997,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" s="38" t="s">
-        <v>1640</v>
+        <v>1649</v>
       </c>
       <c r="B80" t="s">
         <v>1387</v>
@@ -21789,7 +22024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P81">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21798,9 +22033,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" s="38" t="s">
-        <v>1641</v>
+        <v>1648</v>
       </c>
       <c r="B82" t="s">
         <v>1389</v>
@@ -21818,8 +22053,14 @@
       <c r="Q82">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T82" t="s">
+        <v>1642</v>
+      </c>
+      <c r="U82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P83">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21828,7 +22069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>1408</v>
       </c>
@@ -21842,8 +22083,14 @@
       <c r="Q84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T84" t="s">
+        <v>1651</v>
+      </c>
+      <c r="U84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P85">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21852,7 +22099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P86">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21860,10 +22107,16 @@
       <c r="Q86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T86" t="s">
+        <v>1643</v>
+      </c>
+      <c r="U86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="38" t="s">
-        <v>1642</v>
+        <v>1635</v>
       </c>
       <c r="B87" t="s">
         <v>1394</v>
@@ -21885,7 +22138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P88">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21894,7 +22147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P89">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21903,7 +22156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P90">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21911,8 +22164,14 @@
       <c r="Q90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T90" t="s">
+        <v>1652</v>
+      </c>
+      <c r="U90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P91">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21921,7 +22180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P92">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21929,8 +22188,14 @@
       <c r="Q92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T92" t="s">
+        <v>1653</v>
+      </c>
+      <c r="U92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P93">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21939,7 +22204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P94">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21948,7 +22213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P95">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21957,7 +22222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>1403</v>
       </c>
@@ -21969,7 +22234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>1404</v>
       </c>
@@ -21981,7 +22246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P98">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21989,8 +22254,26 @@
       <c r="Q98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="S98" s="33"/>
+      <c r="T98" s="33">
+        <f>COUNTIF(T6:T97, "&lt;&gt;")</f>
+        <v>39</v>
+      </c>
+      <c r="U98" s="33">
+        <f>SUM(U6:U97)</f>
+        <v>192</v>
+      </c>
+      <c r="V98" s="33"/>
+      <c r="W98" s="33"/>
+      <c r="X98" s="33"/>
+      <c r="Y98" s="33"/>
+      <c r="Z98" s="33"/>
+      <c r="AA98" s="33"/>
+      <c r="AB98" s="33"/>
+      <c r="AC98" s="33"/>
+      <c r="AD98" s="33"/>
+    </row>
+    <row r="99" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P99">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21999,7 +22282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P100">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22008,7 +22291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P101">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22017,7 +22300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P102">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22026,7 +22309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P103">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22035,7 +22318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>1411</v>
       </c>
@@ -22047,7 +22330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P105">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22056,7 +22339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>1413</v>
       </c>
@@ -22068,7 +22351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>1412</v>
       </c>
@@ -22083,7 +22366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>1415</v>
       </c>
@@ -22095,7 +22378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P109">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22104,7 +22387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:30" x14ac:dyDescent="0.2">
       <c r="P110">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22113,12 +22396,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:30" x14ac:dyDescent="0.2">
       <c r="Q111">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>1419</v>
       </c>
@@ -22805,7 +23088,7 @@
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" s="38" t="s">
-        <v>1643</v>
+        <v>1637</v>
       </c>
       <c r="B180" t="s">
         <v>1564</v>
@@ -22835,7 +23118,7 @@
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" s="38" t="s">
-        <v>1644</v>
+        <v>1650</v>
       </c>
       <c r="B181" t="s">
         <v>1488</v>
@@ -22856,7 +23139,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" s="38" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="B182" t="s">
         <v>1507</v>
@@ -22873,7 +23156,7 @@
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" s="38" t="s">
-        <v>1646</v>
+        <v>1639</v>
       </c>
       <c r="B183" t="s">
         <v>1438</v>
@@ -23262,7 +23545,7 @@
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="38" t="s">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="B219" t="s">
         <v>1526</v>
@@ -23409,7 +23692,7 @@
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" s="38" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="B232" t="s">
         <v>1539</v>
@@ -23523,7 +23806,7 @@
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="38" t="s">
-        <v>1649</v>
+        <v>1645</v>
       </c>
       <c r="B242" t="s">
         <v>1549</v>
@@ -23726,7 +24009,7 @@
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" s="38" t="s">
-        <v>1650</v>
+        <v>1652</v>
       </c>
       <c r="B261" t="s">
         <v>1568</v>
@@ -23939,7 +24222,7 @@
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A281" s="38" t="s">
-        <v>1651</v>
+        <v>1646</v>
       </c>
       <c r="B281" t="s">
         <v>1587</v>
@@ -23972,7 +24255,7 @@
     </row>
     <row r="283" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A283" s="38" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="B283" t="s">
         <v>1589</v>
@@ -24151,6 +24434,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start working on bubble plot
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -6398,11 +6398,11 @@
   </sheetPr>
   <dimension ref="A1:W200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="111.58"/>
@@ -15327,18 +15327,18 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="111.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="118.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="12.71"/>
@@ -20338,11 +20338,11 @@
   </sheetPr>
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A280" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A280" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B304" activeCellId="0" sqref="B304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="46.42"/>
   </cols>
@@ -21887,11 +21887,11 @@
   </sheetPr>
   <dimension ref="A1:AE299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P115" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V143" activeCellId="0" sqref="V143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P115" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U142" activeCellId="0" sqref="U142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="51.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="46.42"/>

</xml_diff>

<commit_message>
Add tables for topics and venue graphs
- Venue papers table
- Same as pie chart
- Topic description table
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CDB66E-9D3C-4474-BE62-793A82EA4BB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43417F43-1FD0-4C73-9672-F90C9E2C1711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6536,8 +6536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W200"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C183" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G199" sqref="G199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7861,7 +7861,7 @@
         <v>1</v>
       </c>
       <c r="R25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15265,7 +15265,7 @@
       </c>
       <c r="R190" s="22">
         <f>COUNTIFS(R3:R189, "=1")</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S190" s="25"/>
     </row>
@@ -15320,8 +15320,8 @@
         <v>2</v>
       </c>
       <c r="H195" s="2">
-        <f t="shared" ref="H195:H200" si="0">G195/E195</f>
-        <v>0.4</v>
+        <f>(G195/E195)*100</f>
+        <v>40</v>
       </c>
     </row>
     <row r="196" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15344,8 +15344,8 @@
         <v>4</v>
       </c>
       <c r="H196" s="2">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <f>G196/E196*100</f>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="197" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15368,8 +15368,8 @@
         <v>1</v>
       </c>
       <c r="H197" s="2">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <f>G197/E197*100</f>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="198" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15389,11 +15389,11 @@
       </c>
       <c r="G198" s="2">
         <f>COUNTIFS(E3:E189,"JAGI",R3:R189,"&gt;0")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H198" s="2">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <f>G198/E198*100</f>
+        <v>40</v>
       </c>
     </row>
     <row r="199" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15416,8 +15416,8 @@
         <v>79</v>
       </c>
       <c r="H199" s="2">
-        <f t="shared" si="0"/>
-        <v>0.51973684210526316</v>
+        <f>G199/E199*100</f>
+        <v>51.973684210526315</v>
       </c>
     </row>
     <row r="200" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15434,11 +15434,11 @@
       </c>
       <c r="G200" s="26">
         <f>SUM(G195:G199)</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H200" s="2">
-        <f t="shared" si="0"/>
-        <v>0.49732620320855614</v>
+        <f>G200/E200*100</f>
+        <v>49.19786096256685</v>
       </c>
     </row>
   </sheetData>
@@ -15461,8 +15461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20468,7 +20468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A283" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B304" sqref="B304"/>
     </sheetView>
   </sheetViews>
@@ -22009,8 +22009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X166" sqref="X166"/>
+    <sheetView tabSelected="1" topLeftCell="P136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X139" sqref="X139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23250,7 +23250,7 @@
     </row>
     <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P49" s="2">
-        <f t="shared" ref="P49:P80" si="2">COUNTIF(B49:O49,"&lt;&gt;")</f>
+        <f t="shared" ref="P49:P76" si="2">COUNTIF(B49:O49,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q49" s="2">
@@ -25314,7 +25314,7 @@
         <v>1664</v>
       </c>
       <c r="P176" s="2">
-        <f t="shared" ref="P176:P207" si="6">COUNTIF(B176:O176,"&lt;&gt;")</f>
+        <f t="shared" ref="P176:P177" si="6">COUNTIF(B176:O176,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="Q176" s="2">
@@ -26141,7 +26141,7 @@
     </row>
     <row r="249" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P249" s="2">
-        <f t="shared" ref="P249:P280" si="9">COUNTIF(B249:O249,"&lt;&gt;")</f>
+        <f t="shared" ref="P249:P256" si="9">COUNTIF(B249:O249,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q249" s="2">

</xml_diff>

<commit_message>
Update topic freq chart to have yearly colors
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43417F43-1FD0-4C73-9672-F90C9E2C1711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FE5B69-AAB9-43E2-8477-643822E4B3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Results" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3941" uniqueCount="1892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="1893">
   <si>
     <t>Material search results</t>
   </si>
@@ -5714,6 +5714,9 @@
   </si>
   <si>
     <t>AGI research</t>
+  </si>
+  <si>
+    <t>&lt;-- This is just for counting specific categories</t>
   </si>
 </sst>
 </file>
@@ -15461,8 +15464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="M69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20396,6 +20399,13 @@
       <c r="M95" s="22">
         <f>COUNTIF(M3:M94,"&lt;&gt;")</f>
         <v>92</v>
+      </c>
+      <c r="Q95" s="22">
+        <f>COUNTIF(Q3:Q94,"*22*")</f>
+        <v>4</v>
+      </c>
+      <c r="R95" s="22" t="s">
+        <v>1892</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22009,7 +22019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="P136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="X139" sqref="X139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Continue work on topic description chapter
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FE5B69-AAB9-43E2-8477-643822E4B3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075FFDD1-A83C-4644-815D-B3F9C5DB6128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3943" uniqueCount="1894">
   <si>
     <t>Material search results</t>
   </si>
@@ -5717,6 +5717,9 @@
   </si>
   <si>
     <t>&lt;-- This is just for counting specific categories</t>
+  </si>
+  <si>
+    <t>WHY IS THIS IN AI SAFETY? __&gt; change 17, 14 to 14, 21</t>
   </si>
 </sst>
 </file>
@@ -5731,7 +5734,7 @@
     <numFmt numFmtId="168" formatCode="0%"/>
     <numFmt numFmtId="169" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5795,6 +5798,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -6028,7 +6037,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -6127,6 +6136,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent 1 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -15464,8 +15474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q95" sqref="Q95"/>
+    <sheetView tabSelected="1" topLeftCell="L43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18326,8 +18336,11 @@
       <c r="P55" s="2" t="s">
         <v>1374</v>
       </c>
-      <c r="Q55" s="2" t="s">
+      <c r="Q55" s="52" t="s">
         <v>1375</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>1893</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20466,7 +20479,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -22020,7 +22033,7 @@
   <dimension ref="A1:AE299"/>
   <sheetViews>
     <sheetView topLeftCell="P136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X139" sqref="X139"/>
+      <selection activeCell="W163" sqref="W163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add text on time trends, topic relations
- Change heatmap to not draw zeroes
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D31C8BD-69CB-43F7-9215-0B4E48CA3308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCE440-4AFD-485F-A529-D5ED26F82EAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15473,8 +15473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q55"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20405,6 +20405,10 @@
         <f>COUNT(A3:A94)</f>
         <v>92</v>
       </c>
+      <c r="D95" s="22">
+        <f>COUNTIF(D3:D94,"2019")</f>
+        <v>13</v>
+      </c>
       <c r="E95" s="23"/>
       <c r="F95" s="24"/>
       <c r="H95" s="30"/>
@@ -20490,8 +20494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView topLeftCell="A283" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B304" sqref="B304"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add country info to papers
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCE440-4AFD-485F-A529-D5ED26F82EAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19892EA3-306F-48FA-B0E9-3E3CD365770E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3943" uniqueCount="1894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4039" uniqueCount="1943">
   <si>
     <t>Material search results</t>
   </si>
@@ -5720,6 +5720,153 @@
   </si>
   <si>
     <t>14, 21</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Canada, USA, UK</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Singapore, Canada, USA, China</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Sweden, USA, Switzerland</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>France, UK</t>
+  </si>
+  <si>
+    <t>Iceland, USA</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Germany, Netherlands</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Austria, USA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Russia, Netherlands</t>
+  </si>
+  <si>
+    <t>Iceland, Netherlands, USA</t>
+  </si>
+  <si>
+    <t>USA, Canada</t>
+  </si>
+  <si>
+    <t>Netherlands, USA, Russia</t>
+  </si>
+  <si>
+    <t>USA, Austria</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>China, USA</t>
+  </si>
+  <si>
+    <t>Iceland, France</t>
+  </si>
+  <si>
+    <t>China, USA, Ethiopia</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Iceland, Switzerland</t>
+  </si>
+  <si>
+    <t>Iceland, Netherlands</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Canada, USA</t>
+  </si>
+  <si>
+    <t>USA, Russia, Austria</t>
+  </si>
+  <si>
+    <t>Australia, Sweden</t>
+  </si>
+  <si>
+    <t>USA, UK</t>
+  </si>
+  <si>
+    <t>Netherlands, China</t>
+  </si>
+  <si>
+    <t>Russia, France</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Austria, USA, UK</t>
+  </si>
+  <si>
+    <t>Netherlands, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -6036,7 +6183,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -6136,6 +6283,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent 1 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -15471,10 +15619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R1048576"/>
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15494,9 +15642,10 @@
     <col min="15" max="15" width="17" style="2" customWidth="1"/>
     <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="15.140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1195</v>
       </c>
@@ -15504,7 +15653,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -15559,8 +15708,14 @@
       <c r="R2" s="8" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S2" s="8" t="s">
+        <v>1894</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -15612,8 +15767,11 @@
       <c r="Q3" s="2" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>5</v>
       </c>
@@ -15665,8 +15823,11 @@
       <c r="Q4" s="2" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>6</v>
       </c>
@@ -15721,8 +15882,11 @@
       <c r="R5" s="1" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S5" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>8</v>
       </c>
@@ -15774,8 +15938,11 @@
       <c r="Q6" s="2" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="2" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -15824,8 +15991,17 @@
       <c r="Q7" s="2" t="s">
         <v>1221</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>1942</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>1194</v>
+      </c>
+      <c r="T7" s="53" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>17</v>
       </c>
@@ -15874,8 +16050,11 @@
       <c r="Q8" s="2" t="s">
         <v>1224</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>19</v>
       </c>
@@ -15927,8 +16106,11 @@
       <c r="Q9" s="2" t="s">
         <v>1229</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>24</v>
       </c>
@@ -15977,8 +16159,11 @@
       <c r="Q10" s="2" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>25</v>
       </c>
@@ -16027,8 +16212,11 @@
       <c r="Q11" s="2" t="s">
         <v>1237</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>26</v>
       </c>
@@ -16077,8 +16265,11 @@
       <c r="Q12" s="2" t="s">
         <v>1237</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>27</v>
       </c>
@@ -16127,8 +16318,11 @@
       <c r="Q13" s="2" t="s">
         <v>1242</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>28</v>
       </c>
@@ -16177,8 +16371,11 @@
       <c r="Q14" s="2" t="s">
         <v>1245</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>34</v>
       </c>
@@ -16227,8 +16424,11 @@
       <c r="Q15" s="2" t="s">
         <v>1249</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>36</v>
       </c>
@@ -16280,8 +16480,11 @@
       <c r="Q16" s="2" t="s">
         <v>1253</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>37</v>
       </c>
@@ -16333,8 +16536,11 @@
       <c r="Q17" s="2" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>38</v>
       </c>
@@ -16386,8 +16592,11 @@
       <c r="Q18" s="2" t="s">
         <v>1261</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S18" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>39</v>
       </c>
@@ -16439,8 +16648,11 @@
       <c r="Q19" s="2" t="s">
         <v>1264</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>40</v>
       </c>
@@ -16495,8 +16707,11 @@
       <c r="R20" s="2" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S20" s="2" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>41</v>
       </c>
@@ -16548,8 +16763,11 @@
       <c r="Q21" s="2" t="s">
         <v>1273</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S21" s="2" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>42</v>
       </c>
@@ -16601,8 +16819,11 @@
       <c r="Q22" s="2" t="s">
         <v>1276</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S22" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>43</v>
       </c>
@@ -16654,8 +16875,11 @@
       <c r="Q23" s="2" t="s">
         <v>1278</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S23" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>44</v>
       </c>
@@ -16707,8 +16931,11 @@
       <c r="Q24" s="2" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S24" s="2" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>45</v>
       </c>
@@ -16760,8 +16987,11 @@
       <c r="R25" s="1" t="s">
         <v>1283</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S25" s="2" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>46</v>
       </c>
@@ -16810,8 +17040,11 @@
       <c r="Q26" s="2" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S26" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>47</v>
       </c>
@@ -16863,8 +17096,11 @@
       <c r="Q27" s="2" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S27" s="2" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>48</v>
       </c>
@@ -16916,8 +17152,11 @@
       <c r="Q28" s="2" t="s">
         <v>1293</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S28" s="2" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>49</v>
       </c>
@@ -16966,8 +17205,11 @@
       <c r="Q29" s="2" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="2" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>50</v>
       </c>
@@ -17019,8 +17261,11 @@
       <c r="Q30" s="2" t="s">
         <v>1229</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S30" s="2" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>51</v>
       </c>
@@ -17072,8 +17317,11 @@
       <c r="Q31" s="2" t="s">
         <v>1278</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S31" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>52</v>
       </c>
@@ -17125,8 +17373,11 @@
       <c r="Q32" s="2" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S32" s="2" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>54</v>
       </c>
@@ -17178,8 +17429,11 @@
       <c r="Q33" s="2" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S33" s="2" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <v>55</v>
       </c>
@@ -17231,8 +17485,11 @@
       <c r="Q34" s="2" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S34" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <v>56</v>
       </c>
@@ -17284,8 +17541,11 @@
       <c r="Q35" s="2" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S35" s="2" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>57</v>
       </c>
@@ -17337,8 +17597,11 @@
       <c r="Q36" s="2" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S36" s="2" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
         <v>58</v>
       </c>
@@ -17390,8 +17653,11 @@
       <c r="Q37" s="2" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S37" s="2" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <v>59</v>
       </c>
@@ -17443,8 +17709,11 @@
       <c r="Q38" s="2" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S38" s="2" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
         <v>61</v>
       </c>
@@ -17493,8 +17762,11 @@
       <c r="Q39" s="2" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S39" s="2" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>62</v>
       </c>
@@ -17546,8 +17818,11 @@
       <c r="Q40" s="2" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S40" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
         <v>63</v>
       </c>
@@ -17599,8 +17874,11 @@
       <c r="Q41" s="2" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S41" s="2" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>64</v>
       </c>
@@ -17652,8 +17930,11 @@
       <c r="Q42" s="2" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S42" s="2" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
         <v>65</v>
       </c>
@@ -17705,8 +17986,11 @@
       <c r="Q43" s="29" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S43" s="29" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>67</v>
       </c>
@@ -17758,8 +18042,11 @@
       <c r="Q44" s="2" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S44" s="2" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="13">
         <v>68</v>
       </c>
@@ -17814,8 +18101,11 @@
       <c r="R45" s="2" t="s">
         <v>1341</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S45" s="2" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <v>69</v>
       </c>
@@ -17864,8 +18154,11 @@
       <c r="Q46" s="2" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S46" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
         <v>71</v>
       </c>
@@ -17917,8 +18210,11 @@
       <c r="Q47" s="2" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S47" s="2" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13">
         <v>72</v>
       </c>
@@ -17967,8 +18263,11 @@
       <c r="Q48" s="2" t="s">
         <v>1349</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="13">
         <v>73</v>
       </c>
@@ -18017,8 +18316,11 @@
       <c r="Q49" s="2" t="s">
         <v>1355</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S49" s="2" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="13">
         <v>75</v>
       </c>
@@ -18073,8 +18375,11 @@
       <c r="R50" s="1" t="s">
         <v>1360</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S50" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
         <v>78</v>
       </c>
@@ -18126,8 +18431,11 @@
       <c r="Q51" s="2" t="s">
         <v>1365</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S51" s="2" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13">
         <v>80</v>
       </c>
@@ -18179,8 +18487,11 @@
       <c r="Q52" s="2" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S52" s="2" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13">
         <v>81</v>
       </c>
@@ -18229,8 +18540,11 @@
       <c r="Q53" s="2" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S53" s="2" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13">
         <v>82</v>
       </c>
@@ -18285,8 +18599,11 @@
       <c r="R54" s="2" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S54" s="2" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13">
         <v>85</v>
       </c>
@@ -18341,8 +18658,11 @@
       <c r="R55" s="2" t="s">
         <v>1892</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S55" s="2" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13">
         <v>86</v>
       </c>
@@ -18394,8 +18714,11 @@
       <c r="Q56" s="2" t="s">
         <v>1378</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S56" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="13">
         <v>87</v>
       </c>
@@ -18450,8 +18773,11 @@
       <c r="R57" s="2" t="s">
         <v>1380</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S57" s="2" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="13">
         <v>88</v>
       </c>
@@ -18503,8 +18829,11 @@
       <c r="Q58" s="2" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S58" s="2" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13">
         <v>89</v>
       </c>
@@ -18556,8 +18885,11 @@
       <c r="Q59" s="2" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S59" s="2" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13">
         <v>90</v>
       </c>
@@ -18609,8 +18941,11 @@
       <c r="Q60" s="2" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S60" s="2" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
         <v>91</v>
       </c>
@@ -18662,8 +18997,11 @@
       <c r="Q61" s="2" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S61" s="2" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13">
         <v>92</v>
       </c>
@@ -18715,8 +19053,11 @@
       <c r="Q62" s="2" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S62" s="2" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13">
         <v>94</v>
       </c>
@@ -18768,8 +19109,11 @@
       <c r="Q63" s="2" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S63" s="2" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="13">
         <v>97</v>
       </c>
@@ -18821,8 +19165,11 @@
       <c r="Q64" s="2" t="s">
         <v>1400</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S64" s="2" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13">
         <v>98</v>
       </c>
@@ -18874,8 +19221,11 @@
       <c r="Q65" s="2" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S65" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="13">
         <v>99</v>
       </c>
@@ -18927,8 +19277,11 @@
       <c r="Q66" s="2" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S66" s="2" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13">
         <v>100</v>
       </c>
@@ -18977,8 +19330,11 @@
       <c r="Q67" s="2" t="s">
         <v>1410</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S67" s="2" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="13">
         <v>101</v>
       </c>
@@ -19030,8 +19386,11 @@
       <c r="Q68" s="2" t="s">
         <v>1293</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S68" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="13">
         <v>103</v>
       </c>
@@ -19086,8 +19445,11 @@
       <c r="R69" s="2" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S69" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="13">
         <v>104</v>
       </c>
@@ -19139,8 +19501,11 @@
       <c r="Q70" s="2" t="s">
         <v>1232</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S70" s="2" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="13">
         <v>105</v>
       </c>
@@ -19192,8 +19557,11 @@
       <c r="Q71" s="2" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S71" s="2" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="13">
         <v>106</v>
       </c>
@@ -19245,8 +19613,11 @@
       <c r="Q72" s="2" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S72" s="2" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="13">
         <v>107</v>
       </c>
@@ -19298,8 +19669,11 @@
       <c r="Q73" s="2" t="s">
         <v>1431</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S73" s="2" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="13">
         <v>112</v>
       </c>
@@ -19351,8 +19725,11 @@
       <c r="Q74" s="2" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S74" s="2" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="13">
         <v>114</v>
       </c>
@@ -19404,8 +19781,11 @@
       <c r="Q75" s="2" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S75" s="2" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="13">
         <v>115</v>
       </c>
@@ -19457,8 +19837,11 @@
       <c r="Q76" s="2" t="s">
         <v>1245</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S76" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="13">
         <v>117</v>
       </c>
@@ -19510,8 +19893,11 @@
       <c r="Q77" s="2" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S77" s="2" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="13">
         <v>118</v>
       </c>
@@ -19560,8 +19946,11 @@
       <c r="Q78" s="2" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S78" s="2" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="13">
         <v>121</v>
       </c>
@@ -19610,8 +19999,11 @@
       <c r="Q79" s="2" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S79" s="2" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="13">
         <v>124</v>
       </c>
@@ -19663,8 +20055,11 @@
       <c r="Q80" s="2" t="s">
         <v>1449</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S80" s="2" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="13">
         <v>127</v>
       </c>
@@ -19716,8 +20111,11 @@
       <c r="Q81" s="2" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S81" s="2" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="13">
         <v>128</v>
       </c>
@@ -19769,8 +20167,11 @@
       <c r="Q82" s="2" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S82" s="2" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="13">
         <v>131</v>
       </c>
@@ -19822,8 +20223,11 @@
       <c r="Q83" s="2" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S83" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="13">
         <v>132</v>
       </c>
@@ -19872,8 +20276,11 @@
       <c r="Q84" s="2" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S84" s="2" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="13">
         <v>134</v>
       </c>
@@ -19925,8 +20332,11 @@
       <c r="Q85" s="2" t="s">
         <v>1464</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S85" s="2" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="13">
         <v>138</v>
       </c>
@@ -19978,8 +20388,11 @@
       <c r="Q86" s="2" t="s">
         <v>1468</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S86" s="2" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="13">
         <v>139</v>
       </c>
@@ -20031,8 +20444,11 @@
       <c r="Q87" s="2" t="s">
         <v>1245</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S87" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="13">
         <v>141</v>
       </c>
@@ -20084,8 +20500,11 @@
       <c r="Q88" s="2" t="s">
         <v>1245</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S88" s="2" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="13">
         <v>144</v>
       </c>
@@ -20137,8 +20556,11 @@
       <c r="Q89" s="2" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S89" s="2" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="13">
         <v>145</v>
       </c>
@@ -20190,8 +20612,11 @@
       <c r="R90" s="2" t="s">
         <v>1478</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S90" s="2" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="13">
         <v>147</v>
       </c>
@@ -20243,8 +20668,11 @@
       <c r="Q91" s="2" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S91" s="2" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13">
         <v>164</v>
       </c>
@@ -20296,8 +20724,11 @@
       <c r="Q92" s="2" t="s">
         <v>1229</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S92" s="2" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13">
         <v>174</v>
       </c>
@@ -20349,8 +20780,11 @@
       <c r="Q93" s="2" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S93" s="2" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13">
         <v>185</v>
       </c>
@@ -20399,8 +20833,11 @@
       <c r="Q94" s="2" t="s">
         <v>1485</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S94" s="2" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="21">
         <f>COUNT(A3:A94)</f>
         <v>92</v>
@@ -20424,7 +20861,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13"/>
     </row>
     <row r="99" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change czech to czech republic
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19892EA3-306F-48FA-B0E9-3E3CD365770E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0050841F-7590-4DD6-9379-AA02CBB00F51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5743,9 +5743,6 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Czech</t>
-  </si>
-  <si>
     <t>Sweden, USA, Switzerland</t>
   </si>
   <si>
@@ -5867,6 +5864,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
   </si>
 </sst>
 </file>
@@ -15622,7 +15622,7 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15992,7 +15992,7 @@
         <v>1221</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>1194</v>
@@ -16160,7 +16160,7 @@
         <v>1233</v>
       </c>
       <c r="S10" t="s">
-        <v>1901</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16213,7 +16213,7 @@
         <v>1237</v>
       </c>
       <c r="S11" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16266,7 +16266,7 @@
         <v>1237</v>
       </c>
       <c r="S12" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16319,7 +16319,7 @@
         <v>1242</v>
       </c>
       <c r="S13" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16481,7 +16481,7 @@
         <v>1253</v>
       </c>
       <c r="S16" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16537,7 +16537,7 @@
         <v>1257</v>
       </c>
       <c r="S17" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16593,7 +16593,7 @@
         <v>1261</v>
       </c>
       <c r="S18" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16649,7 +16649,7 @@
         <v>1264</v>
       </c>
       <c r="S19" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16708,7 +16708,7 @@
         <v>1269</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16764,7 +16764,7 @@
         <v>1273</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16932,7 +16932,7 @@
         <v>1280</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16988,7 +16988,7 @@
         <v>1283</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17097,7 +17097,7 @@
         <v>1291</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17153,7 +17153,7 @@
         <v>1293</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17206,7 +17206,7 @@
         <v>1257</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17262,7 +17262,7 @@
         <v>1229</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17374,7 +17374,7 @@
         <v>1291</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17430,7 +17430,7 @@
         <v>1302</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17542,7 +17542,7 @@
         <v>1308</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17598,7 +17598,7 @@
         <v>1310</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17654,7 +17654,7 @@
         <v>1313</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17710,7 +17710,7 @@
         <v>1316</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17763,7 +17763,7 @@
         <v>1319</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17875,7 +17875,7 @@
         <v>1301</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17931,7 +17931,7 @@
         <v>1327</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17987,7 +17987,7 @@
         <v>1331</v>
       </c>
       <c r="S43" s="29" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18043,7 +18043,7 @@
         <v>1335</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18102,7 +18102,7 @@
         <v>1341</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18211,7 +18211,7 @@
         <v>1345</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18317,7 +18317,7 @@
         <v>1355</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18432,7 +18432,7 @@
         <v>1365</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18488,7 +18488,7 @@
         <v>1286</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18541,7 +18541,7 @@
         <v>1308</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18600,7 +18600,7 @@
         <v>1371</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18659,7 +18659,7 @@
         <v>1892</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18774,7 +18774,7 @@
         <v>1380</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18830,7 +18830,7 @@
         <v>1257</v>
       </c>
       <c r="S58" s="2" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18886,7 +18886,7 @@
         <v>1310</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18942,7 +18942,7 @@
         <v>1388</v>
       </c>
       <c r="S60" s="2" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="61" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18998,7 +18998,7 @@
         <v>1233</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>1901</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="62" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19054,7 +19054,7 @@
         <v>1358</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="63" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19110,7 +19110,7 @@
         <v>1396</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19166,7 +19166,7 @@
         <v>1400</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19278,7 +19278,7 @@
         <v>1286</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19331,7 +19331,7 @@
         <v>1410</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19502,7 +19502,7 @@
         <v>1232</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19558,7 +19558,7 @@
         <v>1211</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19614,7 +19614,7 @@
         <v>1428</v>
       </c>
       <c r="S72" s="2" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19670,7 +19670,7 @@
         <v>1431</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="74" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19726,7 +19726,7 @@
         <v>1343</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19782,7 +19782,7 @@
         <v>1404</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19894,7 +19894,7 @@
         <v>1335</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19947,7 +19947,7 @@
         <v>1286</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20000,7 +20000,7 @@
         <v>1291</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="80" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20056,7 +20056,7 @@
         <v>1449</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20112,7 +20112,7 @@
         <v>1453</v>
       </c>
       <c r="S81" s="2" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="82" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20168,7 +20168,7 @@
         <v>1301</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20277,7 +20277,7 @@
         <v>1460</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="85" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20333,7 +20333,7 @@
         <v>1464</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="86" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20389,7 +20389,7 @@
         <v>1468</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="87" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20501,7 +20501,7 @@
         <v>1245</v>
       </c>
       <c r="S88" s="2" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="89" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20557,7 +20557,7 @@
         <v>1475</v>
       </c>
       <c r="S89" s="2" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="90" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20613,7 +20613,7 @@
         <v>1478</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="91" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20669,7 +20669,7 @@
         <v>1310</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="92" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20725,7 +20725,7 @@
         <v>1229</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="93" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20781,7 +20781,7 @@
         <v>1310</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="94" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Create initial bubble map with plotly
- Numbers and colors need tweaking
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0050841F-7590-4DD6-9379-AA02CBB00F51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A721A190-3806-4071-8344-22A2A9D45446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15622,7 +15622,7 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edit table, text on publications' volumes
</commit_message>
<xml_diff>
--- a/gradu/material/final_results.xlsx
+++ b/gradu/material/final_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A721A190-3806-4071-8344-22A2A9D45446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955C0EE2-A819-4368-8336-207290177BD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Results" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4039" uniqueCount="1943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="1944">
   <si>
     <t>Material search results</t>
   </si>
@@ -5867,6 +5867,9 @@
   </si>
   <si>
     <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Total papers during the period</t>
   </si>
 </sst>
 </file>
@@ -5881,7 +5884,7 @@
     <numFmt numFmtId="168" formatCode="0%"/>
     <numFmt numFmtId="169" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5947,6 +5950,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -6183,7 +6192,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -6284,6 +6293,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent 1 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -6696,8 +6706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W200"/>
   <sheetViews>
-    <sheetView topLeftCell="C183" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G199" sqref="G199"/>
+    <sheetView tabSelected="1" topLeftCell="C183" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H199" sqref="H199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15432,12 +15442,12 @@
     <row r="191" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="13"/>
     </row>
-    <row r="193" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="2" t="s">
         <v>1188</v>
       </c>
     </row>
-    <row r="194" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="1" t="s">
         <v>1189</v>
       </c>
@@ -15459,8 +15469,11 @@
       <c r="H194" s="1" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="195" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I194" s="54" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="14" t="s">
         <v>28</v>
       </c>
@@ -15483,8 +15496,11 @@
         <f>(G195/E195)*100</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="196" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I195" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="196" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="15" t="s">
         <v>66</v>
       </c>
@@ -15507,8 +15523,11 @@
         <f>G196/E196*100</f>
         <v>33.333333333333329</v>
       </c>
-    </row>
-    <row r="197" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I196" s="2">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="16" t="s">
         <v>145</v>
       </c>
@@ -15531,8 +15550,11 @@
         <f>G197/E197*100</f>
         <v>33.333333333333329</v>
       </c>
-    </row>
-    <row r="198" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I197" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="17" t="s">
         <v>167</v>
       </c>
@@ -15555,8 +15577,11 @@
         <f>G198/E198*100</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="199" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I198" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="19" t="s">
         <v>250</v>
       </c>
@@ -15579,8 +15604,11 @@
         <f>G199/E199*100</f>
         <v>51.973684210526315</v>
       </c>
-    </row>
-    <row r="200" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I199" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="26"/>
       <c r="C200" s="26"/>
       <c r="D200" s="26"/>
@@ -15596,9 +15624,13 @@
         <f>SUM(G195:G199)</f>
         <v>92</v>
       </c>
-      <c r="H200" s="2">
+      <c r="H200" s="32">
         <f>G200/E200*100</f>
         <v>49.19786096256685</v>
+      </c>
+      <c r="I200" s="32">
+        <f>SUM(I195:I199)</f>
+        <v>4784</v>
       </c>
     </row>
   </sheetData>
@@ -15621,8 +15653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="J94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M108" sqref="M108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20910,10 +20942,28 @@
         <v>1488</v>
       </c>
     </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M108"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M109"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M110"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M111"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M112"/>
+    </row>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" sqref="E10:E96 E101" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" sqref="E10:E96 E101 M111:M112" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"JAGI,AIJ,JAIR,ICAGI,IJCAI,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22472,7 +22522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE299"/>
   <sheetViews>
-    <sheetView topLeftCell="P136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="P160" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W163" sqref="W163"/>
     </sheetView>
   </sheetViews>

</xml_diff>